<commit_message>
Updated database & beginning Audio Options dialog.
</commit_message>
<xml_diff>
--- a/Research/Instructions/Instructions New NES.xlsx
+++ b/Research/Instructions/Instructions New NES.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Projects\BeesNES\Research\Instructions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA0BC8F-4068-480F-B1AE-8A404579ECBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{530D3D9D-A266-43A7-90EE-365163A4F810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="14310" yWindow="1380" windowWidth="28800" windowHeight="18765" xr2:uid="{7ED93F2B-FF78-48E4-8428-9E2E36877943}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{7ED93F2B-FF78-48E4-8428-9E2E36877943}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$4979</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$5075</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="106">
+  <futureMetadata name="XLRICHVALUE" count="108">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -786,8 +786,22 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="106"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="107"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="106">
+  <valueMetadata count="108">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -1106,12 +1120,18 @@
     <bk>
       <rc t="1" v="105"/>
     </bk>
+    <bk>
+      <rc t="1" v="106"/>
+    </bk>
+    <bk>
+      <rc t="1" v="107"/>
+    </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2615" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2681" uniqueCount="270">
   <si>
     <t>BRK (00)</t>
   </si>
@@ -5969,6 +5989,174 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <t>ADC (69)</t>
+  </si>
+  <si>
+    <t>ROR (6A)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &gt;&gt; 1) | Tmp.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Set </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> if low bit of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is set.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Set </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Z</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> based off </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>ARR (6B)</t>
   </si>
 </sst>
 </file>
@@ -6261,6 +6449,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -6274,13 +6465,10 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6477,7 +6665,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="106">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="108">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -6902,6 +7090,14 @@
     <v>105</v>
     <v>5</v>
   </rv>
+  <rv s="0">
+    <v>106</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>107</v>
+    <v>5</v>
+  </rv>
 </rvData>
 </file>
 
@@ -7022,6 +7218,8 @@
   <rel r:id="rId104"/>
   <rel r:id="rId105"/>
   <rel r:id="rId106"/>
+  <rel r:id="rId107"/>
+  <rel r:id="rId108"/>
 </richValueRels>
 </file>
 
@@ -7342,10 +7540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236A51FB-68FA-4644-A8C6-D47AA32EBCC5}">
-  <dimension ref="B1:F4912"/>
+  <dimension ref="B1:F5049"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4893" zoomScale="115" zoomScaleNormal="55" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="E4895" sqref="E4895"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5007" zoomScale="115" zoomScaleNormal="55" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="C5030" sqref="C5030"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7540,14 +7738,14 @@
         <v>7.1</v>
       </c>
       <c r="D20" s="10"/>
-      <c r="E20" s="47" t="s">
+      <c r="E20" s="48" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="47"/>
+      <c r="E21" s="48"/>
     </row>
     <row r="22" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="9">
@@ -7568,42 +7766,42 @@
       <c r="E23" s="17"/>
     </row>
     <row r="25" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="50" t="s">
+      <c r="B25" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
+      <c r="C25" s="49"/>
+      <c r="D25" s="49"/>
+      <c r="E25" s="49"/>
     </row>
     <row r="26" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="50"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="50"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
     </row>
     <row r="27" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="50"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="49"/>
+      <c r="E27" s="49"/>
     </row>
     <row r="28" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
     </row>
     <row r="29" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
     </row>
     <row r="30" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="50"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
-      <c r="E30" s="50"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
     </row>
     <row r="31" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C31" s="43" t="e" vm="1">
@@ -7695,10 +7893,10 @@
     </row>
     <row r="48" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C48" s="21"/>
-      <c r="D48" s="44" t="s">
+      <c r="D48" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="E48" s="45"/>
+      <c r="E48" s="46"/>
     </row>
     <row r="49" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C49" s="7" t="s">
@@ -7852,12 +8050,12 @@
       <c r="E64" s="14"/>
     </row>
     <row r="65" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="46" t="s">
+      <c r="B65" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C65" s="46"/>
-      <c r="D65" s="46"/>
-      <c r="E65" s="46"/>
+      <c r="C65" s="47"/>
+      <c r="D65" s="47"/>
+      <c r="E65" s="47"/>
     </row>
     <row r="66" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C66" s="24"/>
@@ -7949,10 +8147,10 @@
     </row>
     <row r="95" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C95" s="21"/>
-      <c r="D95" s="44" t="s">
+      <c r="D95" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E95" s="45"/>
+      <c r="E95" s="46"/>
     </row>
     <row r="96" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C96" s="7" t="s">
@@ -8160,10 +8358,10 @@
     </row>
     <row r="142" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C142" s="21"/>
-      <c r="D142" s="44" t="s">
+      <c r="D142" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="E142" s="45"/>
+      <c r="E142" s="46"/>
     </row>
     <row r="143" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C143" s="7" t="s">
@@ -8304,14 +8502,14 @@
         <v>7.1</v>
       </c>
       <c r="D157" s="10"/>
-      <c r="E157" s="47" t="s">
+      <c r="E157" s="48" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="158" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C158" s="9"/>
       <c r="D158" s="10"/>
-      <c r="E158" s="47"/>
+      <c r="E158" s="48"/>
     </row>
     <row r="159" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C159" s="40">
@@ -8352,12 +8550,12 @@
       </c>
     </row>
     <row r="164" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B164" s="46" t="s">
+      <c r="B164" s="47" t="s">
         <v>170</v>
       </c>
-      <c r="C164" s="46"/>
-      <c r="D164" s="46"/>
-      <c r="E164" s="46"/>
+      <c r="C164" s="47"/>
+      <c r="D164" s="47"/>
+      <c r="E164" s="47"/>
     </row>
     <row r="166" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C166" s="43" t="e" vm="4">
@@ -8459,10 +8657,10 @@
     </row>
     <row r="189" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C189" s="21"/>
-      <c r="D189" s="44" t="s">
+      <c r="D189" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="E189" s="45"/>
+      <c r="E189" s="46"/>
     </row>
     <row r="190" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C190" s="7" t="s">
@@ -8611,10 +8809,10 @@
     </row>
     <row r="236" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C236" s="21"/>
-      <c r="D236" s="44" t="s">
+      <c r="D236" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="E236" s="45"/>
+      <c r="E236" s="46"/>
     </row>
     <row r="237" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C237" s="7" t="s">
@@ -8708,12 +8906,12 @@
       </c>
     </row>
     <row r="247" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B247" s="46" t="s">
+      <c r="B247" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C247" s="46"/>
-      <c r="D247" s="46"/>
-      <c r="E247" s="46"/>
+      <c r="C247" s="47"/>
+      <c r="D247" s="47"/>
+      <c r="E247" s="47"/>
     </row>
     <row r="249" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C249" s="43" t="e" vm="6">
@@ -8775,10 +8973,10 @@
     </row>
     <row r="283" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C283" s="21"/>
-      <c r="D283" s="44" t="s">
+      <c r="D283" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="E283" s="45"/>
+      <c r="E283" s="46"/>
     </row>
     <row r="284" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C284" s="7" t="s">
@@ -8865,14 +9063,14 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D292" s="10"/>
-      <c r="E292" s="47" t="s">
+      <c r="E292" s="48" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="293" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C293" s="9"/>
       <c r="D293" s="10"/>
-      <c r="E293" s="47"/>
+      <c r="E293" s="48"/>
     </row>
     <row r="294" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C294" s="40">
@@ -8985,10 +9183,10 @@
     </row>
     <row r="330" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C330" s="21"/>
-      <c r="D330" s="44" t="s">
+      <c r="D330" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="E330" s="45"/>
+      <c r="E330" s="46"/>
     </row>
     <row r="331" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C331" s="7" t="s">
@@ -9075,14 +9273,14 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D339" s="10"/>
-      <c r="E339" s="47" t="s">
+      <c r="E339" s="48" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="340" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C340" s="9"/>
       <c r="D340" s="10"/>
-      <c r="E340" s="47"/>
+      <c r="E340" s="48"/>
     </row>
     <row r="341" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C341" s="40">
@@ -9123,12 +9321,12 @@
       </c>
     </row>
     <row r="346" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B346" s="46" t="s">
+      <c r="B346" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C346" s="46"/>
-      <c r="D346" s="46"/>
-      <c r="E346" s="46"/>
+      <c r="C346" s="47"/>
+      <c r="D346" s="47"/>
+      <c r="E346" s="47"/>
     </row>
     <row r="348" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C348" s="43" t="e" vm="8">
@@ -9205,10 +9403,10 @@
     </row>
     <row r="377" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C377" s="21"/>
-      <c r="D377" s="44" t="s">
+      <c r="D377" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E377" s="45"/>
+      <c r="E377" s="46"/>
     </row>
     <row r="378" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C378" s="7" t="s">
@@ -9357,10 +9555,10 @@
     </row>
     <row r="424" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C424" s="21"/>
-      <c r="D424" s="44" t="s">
+      <c r="D424" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="E424" s="45"/>
+      <c r="E424" s="46"/>
     </row>
     <row r="425" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C425" s="7" t="s">
@@ -9434,12 +9632,12 @@
       </c>
     </row>
     <row r="433" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B433" s="46" t="s">
+      <c r="B433" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C433" s="46"/>
-      <c r="D433" s="46"/>
-      <c r="E433" s="46"/>
+      <c r="C433" s="47"/>
+      <c r="D433" s="47"/>
+      <c r="E433" s="47"/>
     </row>
     <row r="435" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C435" s="43" t="e" vm="10">
@@ -9491,10 +9689,10 @@
     </row>
     <row r="471" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C471" s="21"/>
-      <c r="D471" s="44" t="s">
+      <c r="D471" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E471" s="45"/>
+      <c r="E471" s="46"/>
     </row>
     <row r="472" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C472" s="7" t="s">
@@ -9543,14 +9741,14 @@
         <v>2.1</v>
       </c>
       <c r="D476" s="10"/>
-      <c r="E476" s="47" t="s">
+      <c r="E476" s="48" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="477" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C477" s="9"/>
       <c r="D477" s="10"/>
-      <c r="E477" s="47"/>
+      <c r="E477" s="48"/>
     </row>
     <row r="478" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C478" s="9">
@@ -9573,12 +9771,12 @@
       </c>
     </row>
     <row r="481" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B481" s="46" t="s">
+      <c r="B481" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C481" s="46"/>
-      <c r="D481" s="46"/>
-      <c r="E481" s="46"/>
+      <c r="C481" s="47"/>
+      <c r="D481" s="47"/>
+      <c r="E481" s="47"/>
     </row>
     <row r="483" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C483" s="43" t="e" vm="11">
@@ -9630,10 +9828,10 @@
     </row>
     <row r="518" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C518" s="21"/>
-      <c r="D518" s="44" t="s">
+      <c r="D518" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="E518" s="45"/>
+      <c r="E518" s="46"/>
     </row>
     <row r="519" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C519" s="7" t="s">
@@ -9682,14 +9880,14 @@
         <v>2.1</v>
       </c>
       <c r="D523" s="10"/>
-      <c r="E523" s="47" t="s">
+      <c r="E523" s="48" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="524" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C524" s="9"/>
       <c r="D524" s="10"/>
-      <c r="E524" s="47"/>
+      <c r="E524" s="48"/>
     </row>
     <row r="525" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C525" s="9">
@@ -9712,20 +9910,20 @@
       </c>
     </row>
     <row r="528" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B528" s="46" t="s">
+      <c r="B528" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C528" s="46"/>
-      <c r="D528" s="46"/>
-      <c r="E528" s="46"/>
+      <c r="C528" s="47"/>
+      <c r="D528" s="47"/>
+      <c r="E528" s="47"/>
     </row>
     <row r="529" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B529" s="48" t="s">
+      <c r="B529" s="50" t="s">
         <v>171</v>
       </c>
-      <c r="C529" s="48"/>
-      <c r="D529" s="48"/>
-      <c r="E529" s="48"/>
+      <c r="C529" s="50"/>
+      <c r="D529" s="50"/>
+      <c r="E529" s="50"/>
     </row>
     <row r="531" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C531" s="43" t="e" vm="12">
@@ -9837,11 +10035,11 @@
       <c r="E552" s="43"/>
     </row>
     <row r="553" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C553" s="48" t="s">
+      <c r="C553" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="D553" s="48"/>
-      <c r="E553" s="48"/>
+      <c r="D553" s="50"/>
+      <c r="E553" s="50"/>
     </row>
     <row r="564" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C564" s="1" t="s">
@@ -9856,10 +10054,10 @@
     </row>
     <row r="565" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C565" s="21"/>
-      <c r="D565" s="44" t="s">
+      <c r="D565" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="E565" s="45"/>
+      <c r="E565" s="46"/>
     </row>
     <row r="566" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C566" s="7" t="s">
@@ -10038,10 +10236,10 @@
     </row>
     <row r="612" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C612" s="21"/>
-      <c r="D612" s="44" t="s">
+      <c r="D612" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="E612" s="45"/>
+      <c r="E612" s="46"/>
     </row>
     <row r="613" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C613" s="7" t="s">
@@ -10155,12 +10353,12 @@
       </c>
     </row>
     <row r="625" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B625" s="46" t="s">
+      <c r="B625" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C625" s="46"/>
-      <c r="D625" s="46"/>
-      <c r="E625" s="46"/>
+      <c r="C625" s="47"/>
+      <c r="D625" s="47"/>
+      <c r="E625" s="47"/>
     </row>
     <row r="627" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C627" s="43" t="e" vm="15">
@@ -10227,10 +10425,10 @@
     </row>
     <row r="659" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C659" s="21"/>
-      <c r="D659" s="44" t="s">
+      <c r="D659" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="E659" s="45"/>
+      <c r="E659" s="46"/>
     </row>
     <row r="660" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C660" s="7" t="s">
@@ -10337,14 +10535,14 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D670" s="10"/>
-      <c r="E670" s="47" t="s">
+      <c r="E670" s="48" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="671" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C671" s="9"/>
       <c r="D671" s="10"/>
-      <c r="E671" s="47"/>
+      <c r="E671" s="48"/>
     </row>
     <row r="672" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C672" s="40">
@@ -10467,10 +10665,10 @@
     </row>
     <row r="706" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C706" s="21"/>
-      <c r="D706" s="44" t="s">
+      <c r="D706" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="E706" s="45"/>
+      <c r="E706" s="46"/>
     </row>
     <row r="707" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C707" s="7" t="s">
@@ -10577,14 +10775,14 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D717" s="10"/>
-      <c r="E717" s="47" t="s">
+      <c r="E717" s="48" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="718" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C718" s="9"/>
       <c r="D718" s="10"/>
-      <c r="E718" s="47"/>
+      <c r="E718" s="48"/>
     </row>
     <row r="719" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C719" s="40">
@@ -10625,12 +10823,12 @@
       </c>
     </row>
     <row r="724" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B724" s="46" t="s">
+      <c r="B724" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C724" s="46"/>
-      <c r="D724" s="46"/>
-      <c r="E724" s="46"/>
+      <c r="C724" s="47"/>
+      <c r="D724" s="47"/>
+      <c r="E724" s="47"/>
     </row>
     <row r="726" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C726" s="43" t="e" vm="17">
@@ -10717,10 +10915,10 @@
     </row>
     <row r="753" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C753" s="21"/>
-      <c r="D753" s="44" t="s">
+      <c r="D753" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="E753" s="45"/>
+      <c r="E753" s="46"/>
     </row>
     <row r="754" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C754" s="7" t="s">
@@ -10760,14 +10958,14 @@
       <c r="D757" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E757" s="47" t="s">
+      <c r="E757" s="48" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="758" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C758" s="9"/>
       <c r="D758" s="10"/>
-      <c r="E758" s="47"/>
+      <c r="E758" s="48"/>
     </row>
     <row r="759" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C759" s="9">
@@ -10792,14 +10990,14 @@
         <v>3.1</v>
       </c>
       <c r="D761" s="10"/>
-      <c r="E761" s="47" t="s">
+      <c r="E761" s="48" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="762" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C762" s="9"/>
       <c r="D762" s="10"/>
-      <c r="E762" s="47"/>
+      <c r="E762" s="48"/>
     </row>
     <row r="763" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C763" s="40">
@@ -10991,10 +11189,10 @@
     </row>
     <row r="800" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C800" s="21"/>
-      <c r="D800" s="44" t="s">
+      <c r="D800" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="E800" s="45"/>
+      <c r="E800" s="46"/>
     </row>
     <row r="801" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C801" s="7" t="s">
@@ -11092,14 +11290,14 @@
       <c r="D810" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E810" s="47" t="s">
+      <c r="E810" s="48" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="811" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C811" s="9"/>
       <c r="D811" s="10"/>
-      <c r="E811" s="47"/>
+      <c r="E811" s="48"/>
     </row>
     <row r="812" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C812" s="29">
@@ -11151,12 +11349,12 @@
       </c>
     </row>
     <row r="818" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B818" s="46" t="s">
+      <c r="B818" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C818" s="46"/>
-      <c r="D818" s="46"/>
-      <c r="E818" s="46"/>
+      <c r="C818" s="47"/>
+      <c r="D818" s="47"/>
+      <c r="E818" s="47"/>
     </row>
     <row r="820" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C820" s="43" t="e" vm="21">
@@ -11233,10 +11431,10 @@
     </row>
     <row r="847" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C847" s="21"/>
-      <c r="D847" s="44" t="s">
+      <c r="D847" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E847" s="45"/>
+      <c r="E847" s="46"/>
     </row>
     <row r="848" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C848" s="7" t="s">
@@ -11444,10 +11642,10 @@
     </row>
     <row r="894" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C894" s="21"/>
-      <c r="D894" s="44" t="s">
+      <c r="D894" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="E894" s="45"/>
+      <c r="E894" s="46"/>
     </row>
     <row r="895" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C895" s="7" t="s">
@@ -11592,14 +11790,14 @@
         <v>7.1</v>
       </c>
       <c r="D909" s="10"/>
-      <c r="E909" s="47" t="s">
+      <c r="E909" s="48" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="910" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C910" s="9"/>
       <c r="D910" s="10"/>
-      <c r="E910" s="47"/>
+      <c r="E910" s="48"/>
     </row>
     <row r="911" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C911" s="40">
@@ -11640,12 +11838,12 @@
       </c>
     </row>
     <row r="916" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B916" s="46" t="s">
+      <c r="B916" s="47" t="s">
         <v>170</v>
       </c>
-      <c r="C916" s="46"/>
-      <c r="D916" s="46"/>
-      <c r="E916" s="46"/>
+      <c r="C916" s="47"/>
+      <c r="D916" s="47"/>
+      <c r="E916" s="47"/>
     </row>
     <row r="918" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C918" s="43" t="e" vm="22">
@@ -11747,10 +11945,10 @@
     </row>
     <row r="941" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C941" s="21"/>
-      <c r="D941" s="44" t="s">
+      <c r="D941" s="45" t="s">
         <v>245</v>
       </c>
-      <c r="E941" s="45"/>
+      <c r="E941" s="46"/>
     </row>
     <row r="942" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C942" s="7" t="s">
@@ -11929,10 +12127,10 @@
     </row>
     <row r="988" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C988" s="21"/>
-      <c r="D988" s="44" t="s">
+      <c r="D988" s="45" t="s">
         <v>245</v>
       </c>
-      <c r="E988" s="45"/>
+      <c r="E988" s="46"/>
     </row>
     <row r="989" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C989" s="7" t="s">
@@ -12051,12 +12249,12 @@
       <c r="E1000" s="14"/>
     </row>
     <row r="1001" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1001" s="46" t="s">
+      <c r="B1001" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C1001" s="46"/>
-      <c r="D1001" s="46"/>
-      <c r="E1001" s="46"/>
+      <c r="C1001" s="47"/>
+      <c r="D1001" s="47"/>
+      <c r="E1001" s="47"/>
     </row>
     <row r="1003" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1003" s="43" t="e" vm="24">
@@ -12128,10 +12326,10 @@
     </row>
     <row r="1035" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1035" s="21"/>
-      <c r="D1035" s="44" t="s">
+      <c r="D1035" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="E1035" s="45"/>
+      <c r="E1035" s="46"/>
     </row>
     <row r="1036" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1036" s="7" t="s">
@@ -12238,14 +12436,14 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D1046" s="10"/>
-      <c r="E1046" s="47" t="s">
+      <c r="E1046" s="48" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="1047" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1047" s="9"/>
       <c r="D1047" s="10"/>
-      <c r="E1047" s="47"/>
+      <c r="E1047" s="48"/>
     </row>
     <row r="1048" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1048" s="40">
@@ -12368,10 +12566,10 @@
     </row>
     <row r="1082" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1082" s="21"/>
-      <c r="D1082" s="44" t="s">
+      <c r="D1082" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="E1082" s="45"/>
+      <c r="E1082" s="46"/>
     </row>
     <row r="1083" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1083" s="7" t="s">
@@ -12478,14 +12676,14 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D1093" s="10"/>
-      <c r="E1093" s="47" t="s">
+      <c r="E1093" s="48" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="1094" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1094" s="9"/>
       <c r="D1094" s="10"/>
-      <c r="E1094" s="47"/>
+      <c r="E1094" s="48"/>
     </row>
     <row r="1095" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1095" s="40">
@@ -12526,12 +12724,12 @@
       </c>
     </row>
     <row r="1100" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1100" s="46" t="s">
+      <c r="B1100" s="47" t="s">
         <v>170</v>
       </c>
-      <c r="C1100" s="46"/>
-      <c r="D1100" s="46"/>
-      <c r="E1100" s="46"/>
+      <c r="C1100" s="47"/>
+      <c r="D1100" s="47"/>
+      <c r="E1100" s="47"/>
     </row>
     <row r="1102" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1102" s="43" t="e" vm="26">
@@ -12618,10 +12816,10 @@
     </row>
     <row r="1129" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1129" s="21"/>
-      <c r="D1129" s="44" t="s">
+      <c r="D1129" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E1129" s="45"/>
+      <c r="E1129" s="46"/>
     </row>
     <row r="1130" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1130" s="7" t="s">
@@ -12747,10 +12945,10 @@
     </row>
     <row r="1176" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1176" s="21"/>
-      <c r="D1176" s="44" t="s">
+      <c r="D1176" s="45" t="s">
         <v>247</v>
       </c>
-      <c r="E1176" s="45"/>
+      <c r="E1176" s="46"/>
     </row>
     <row r="1177" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1177" s="7" t="s">
@@ -12830,14 +13028,14 @@
       <c r="D1184" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E1184" s="47" t="s">
+      <c r="E1184" s="48" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="1185" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1185" s="9"/>
       <c r="D1185" s="10"/>
-      <c r="E1185" s="47"/>
+      <c r="E1185" s="48"/>
     </row>
     <row r="1186" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1186" s="29">
@@ -12889,12 +13087,12 @@
       </c>
     </row>
     <row r="1192" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1192" s="46" t="s">
+      <c r="B1192" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C1192" s="46"/>
-      <c r="D1192" s="46"/>
-      <c r="E1192" s="46"/>
+      <c r="C1192" s="47"/>
+      <c r="D1192" s="47"/>
+      <c r="E1192" s="47"/>
     </row>
     <row r="1194" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1194" s="43" t="e" vm="28">
@@ -12971,10 +13169,10 @@
     </row>
     <row r="1223" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1223" s="21"/>
-      <c r="D1223" s="44" t="s">
+      <c r="D1223" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E1223" s="45"/>
+      <c r="E1223" s="46"/>
     </row>
     <row r="1224" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1224" s="7" t="s">
@@ -13093,10 +13291,10 @@
     </row>
     <row r="1270" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1270" s="21"/>
-      <c r="D1270" s="44" t="s">
+      <c r="D1270" s="45" t="s">
         <v>248</v>
       </c>
-      <c r="E1270" s="45"/>
+      <c r="E1270" s="46"/>
     </row>
     <row r="1271" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1271" s="7" t="s">
@@ -13223,14 +13421,14 @@
         <v>6.1</v>
       </c>
       <c r="D1283" s="10"/>
-      <c r="E1283" s="47" t="s">
+      <c r="E1283" s="48" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="1284" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1284" s="9"/>
       <c r="D1284" s="10"/>
-      <c r="E1284" s="47"/>
+      <c r="E1284" s="48"/>
     </row>
     <row r="1285" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1285" s="40">
@@ -13271,12 +13469,12 @@
       </c>
     </row>
     <row r="1290" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1290" s="46" t="s">
+      <c r="B1290" s="47" t="s">
         <v>172</v>
       </c>
-      <c r="C1290" s="46"/>
-      <c r="D1290" s="46"/>
-      <c r="E1290" s="46"/>
+      <c r="C1290" s="47"/>
+      <c r="D1290" s="47"/>
+      <c r="E1290" s="47"/>
     </row>
     <row r="1292" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1292" s="43" t="e" vm="30">
@@ -13368,10 +13566,10 @@
     </row>
     <row r="1317" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1317" s="21"/>
-      <c r="D1317" s="44" t="s">
+      <c r="D1317" s="45" t="s">
         <v>244</v>
       </c>
-      <c r="E1317" s="45"/>
+      <c r="E1317" s="46"/>
     </row>
     <row r="1318" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1318" s="7" t="s">
@@ -13451,14 +13649,14 @@
       <c r="D1325" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E1325" s="47" t="s">
+      <c r="E1325" s="48" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="1326" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1326" s="9"/>
       <c r="D1326" s="10"/>
-      <c r="E1326" s="47"/>
+      <c r="E1326" s="48"/>
     </row>
     <row r="1327" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1327" s="29">
@@ -13575,10 +13773,10 @@
     </row>
     <row r="1364" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1364" s="21"/>
-      <c r="D1364" s="44" t="s">
+      <c r="D1364" s="45" t="s">
         <v>244</v>
       </c>
-      <c r="E1364" s="45"/>
+      <c r="E1364" s="46"/>
     </row>
     <row r="1365" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1365" s="7" t="s">
@@ -13658,14 +13856,14 @@
       <c r="D1372" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E1372" s="47" t="s">
+      <c r="E1372" s="48" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="1373" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1373" s="9"/>
       <c r="D1373" s="10"/>
-      <c r="E1373" s="47"/>
+      <c r="E1373" s="48"/>
     </row>
     <row r="1374" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1374" s="29">
@@ -13722,12 +13920,12 @@
       <c r="E1379" s="14"/>
     </row>
     <row r="1380" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1380" s="46" t="s">
+      <c r="B1380" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C1380" s="46"/>
-      <c r="D1380" s="46"/>
-      <c r="E1380" s="46"/>
+      <c r="C1380" s="47"/>
+      <c r="D1380" s="47"/>
+      <c r="E1380" s="47"/>
     </row>
     <row r="1382" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1382" s="43" t="e" vm="32">
@@ -13804,10 +14002,10 @@
     </row>
     <row r="1411" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1411" s="21"/>
-      <c r="D1411" s="44" t="s">
+      <c r="D1411" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="E1411" s="45"/>
+      <c r="E1411" s="46"/>
     </row>
     <row r="1412" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1412" s="7" t="s">
@@ -13934,14 +14132,14 @@
         <v>6.1</v>
       </c>
       <c r="D1424" s="10"/>
-      <c r="E1424" s="47" t="s">
+      <c r="E1424" s="48" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="1425" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1425" s="9"/>
       <c r="D1425" s="10"/>
-      <c r="E1425" s="47"/>
+      <c r="E1425" s="48"/>
     </row>
     <row r="1426" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1426" s="40">
@@ -14069,10 +14267,10 @@
     </row>
     <row r="1458" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1458" s="21"/>
-      <c r="D1458" s="44" t="s">
+      <c r="D1458" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="E1458" s="45"/>
+      <c r="E1458" s="46"/>
     </row>
     <row r="1459" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1459" s="7" t="s">
@@ -14199,14 +14397,14 @@
         <v>6.1</v>
       </c>
       <c r="D1471" s="10"/>
-      <c r="E1471" s="47" t="s">
+      <c r="E1471" s="48" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="1472" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1472" s="9"/>
       <c r="D1472" s="10"/>
-      <c r="E1472" s="47"/>
+      <c r="E1472" s="48"/>
     </row>
     <row r="1473" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1473" s="40">
@@ -14247,12 +14445,12 @@
       </c>
     </row>
     <row r="1478" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1478" s="46" t="s">
+      <c r="B1478" s="47" t="s">
         <v>170</v>
       </c>
-      <c r="C1478" s="46"/>
-      <c r="D1478" s="46"/>
-      <c r="E1478" s="46"/>
+      <c r="C1478" s="47"/>
+      <c r="D1478" s="47"/>
+      <c r="E1478" s="47"/>
     </row>
     <row r="1480" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1480" s="43" t="e" vm="34">
@@ -14344,10 +14542,10 @@
     </row>
     <row r="1505" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1505" s="21"/>
-      <c r="D1505" s="44" t="s">
+      <c r="D1505" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="E1505" s="45"/>
+      <c r="E1505" s="46"/>
     </row>
     <row r="1506" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1506" s="7" t="s">
@@ -14575,10 +14773,10 @@
     </row>
     <row r="1552" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1552" s="21"/>
-      <c r="D1552" s="44" t="s">
+      <c r="D1552" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="E1552" s="45"/>
+      <c r="E1552" s="46"/>
     </row>
     <row r="1553" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1553" s="7" t="s">
@@ -14731,12 +14929,12 @@
       <c r="E1568" s="14"/>
     </row>
     <row r="1569" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1569" s="46" t="s">
+      <c r="B1569" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C1569" s="46"/>
-      <c r="D1569" s="46"/>
-      <c r="E1569" s="46"/>
+      <c r="C1569" s="47"/>
+      <c r="D1569" s="47"/>
+      <c r="E1569" s="47"/>
     </row>
     <row r="1571" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1571" s="43" t="e" vm="36">
@@ -14823,10 +15021,10 @@
     </row>
     <row r="1599" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1599" s="21"/>
-      <c r="D1599" s="44" t="s">
+      <c r="D1599" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E1599" s="45"/>
+      <c r="E1599" s="46"/>
     </row>
     <row r="1600" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1600" s="7" t="s">
@@ -15034,10 +15232,10 @@
     </row>
     <row r="1646" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1646" s="21"/>
-      <c r="D1646" s="44" t="s">
+      <c r="D1646" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="E1646" s="45"/>
+      <c r="E1646" s="46"/>
     </row>
     <row r="1647" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1647" s="7" t="s">
@@ -15178,19 +15376,19 @@
         <v>7.1</v>
       </c>
       <c r="D1661" s="10"/>
-      <c r="E1661" s="47" t="s">
+      <c r="E1661" s="48" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="1662" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1662" s="9"/>
       <c r="D1662" s="10"/>
-      <c r="E1662" s="47"/>
+      <c r="E1662" s="48"/>
     </row>
     <row r="1663" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1663" s="9"/>
       <c r="D1663" s="10"/>
-      <c r="E1663" s="47"/>
+      <c r="E1663" s="48"/>
     </row>
     <row r="1664" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1664" s="40">
@@ -15231,12 +15429,12 @@
       </c>
     </row>
     <row r="1669" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1669" s="46" t="s">
+      <c r="B1669" s="47" t="s">
         <v>170</v>
       </c>
-      <c r="C1669" s="46"/>
-      <c r="D1669" s="46"/>
-      <c r="E1669" s="46"/>
+      <c r="C1669" s="47"/>
+      <c r="D1669" s="47"/>
+      <c r="E1669" s="47"/>
     </row>
     <row r="1671" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1671" s="43" t="e" vm="37">
@@ -15338,10 +15536,10 @@
     </row>
     <row r="1693" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1693" s="21"/>
-      <c r="D1693" s="44" t="s">
+      <c r="D1693" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="E1693" s="45"/>
+      <c r="E1693" s="46"/>
     </row>
     <row r="1694" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1694" s="7" t="s">
@@ -15506,10 +15704,10 @@
     </row>
     <row r="1740" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1740" s="21"/>
-      <c r="D1740" s="44" t="s">
+      <c r="D1740" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="E1740" s="45"/>
+      <c r="E1740" s="46"/>
     </row>
     <row r="1741" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1741" s="7" t="s">
@@ -15608,12 +15806,12 @@
       <c r="E1750" s="14"/>
     </row>
     <row r="1751" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1751" s="46" t="s">
+      <c r="B1751" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C1751" s="46"/>
-      <c r="D1751" s="46"/>
-      <c r="E1751" s="46"/>
+      <c r="C1751" s="47"/>
+      <c r="D1751" s="47"/>
+      <c r="E1751" s="47"/>
     </row>
     <row r="1753" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1753" s="43" t="e" vm="39">
@@ -15675,10 +15873,10 @@
     </row>
     <row r="1787" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1787" s="21"/>
-      <c r="D1787" s="44" t="s">
+      <c r="D1787" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="E1787" s="45"/>
+      <c r="E1787" s="46"/>
     </row>
     <row r="1788" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1788" s="7" t="s">
@@ -15765,14 +15963,14 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D1796" s="10"/>
-      <c r="E1796" s="47" t="s">
+      <c r="E1796" s="48" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="1797" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1797" s="9"/>
       <c r="D1797" s="10"/>
-      <c r="E1797" s="47"/>
+      <c r="E1797" s="48"/>
     </row>
     <row r="1798" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1798" s="40">
@@ -15885,10 +16083,10 @@
     </row>
     <row r="1834" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1834" s="21"/>
-      <c r="D1834" s="44" t="s">
+      <c r="D1834" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="E1834" s="45"/>
+      <c r="E1834" s="46"/>
     </row>
     <row r="1835" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1835" s="7" t="s">
@@ -15975,19 +16173,19 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D1843" s="10"/>
-      <c r="E1843" s="47" t="s">
+      <c r="E1843" s="48" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="1844" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1844" s="9"/>
       <c r="D1844" s="10"/>
-      <c r="E1844" s="47"/>
+      <c r="E1844" s="48"/>
     </row>
     <row r="1845" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1845" s="9"/>
       <c r="D1845" s="10"/>
-      <c r="E1845" s="47"/>
+      <c r="E1845" s="48"/>
     </row>
     <row r="1846" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1846" s="40">
@@ -16033,12 +16231,12 @@
       <c r="E1850" s="14"/>
     </row>
     <row r="1851" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1851" s="46" t="s">
+      <c r="B1851" s="47" t="s">
         <v>170</v>
       </c>
-      <c r="C1851" s="46"/>
-      <c r="D1851" s="46"/>
-      <c r="E1851" s="46"/>
+      <c r="C1851" s="47"/>
+      <c r="D1851" s="47"/>
+      <c r="E1851" s="47"/>
     </row>
     <row r="1853" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1853" s="43" t="e" vm="41">
@@ -16295,10 +16493,10 @@
     </row>
     <row r="1928" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1928" s="21"/>
-      <c r="D1928" s="44" t="s">
+      <c r="D1928" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="E1928" s="45"/>
+      <c r="E1928" s="46"/>
     </row>
     <row r="1929" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1929" s="7" t="s">
@@ -16377,12 +16575,12 @@
       <c r="E1936" s="14"/>
     </row>
     <row r="1937" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1937" s="46" t="s">
+      <c r="B1937" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C1937" s="46"/>
-      <c r="D1937" s="46"/>
-      <c r="E1937" s="46"/>
+      <c r="C1937" s="47"/>
+      <c r="D1937" s="47"/>
+      <c r="E1937" s="47"/>
     </row>
     <row r="1939" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1939" s="43" t="e" vm="43">
@@ -16434,10 +16632,10 @@
     </row>
     <row r="1975" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1975" s="21"/>
-      <c r="D1975" s="44" t="s">
+      <c r="D1975" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="E1975" s="45"/>
+      <c r="E1975" s="46"/>
     </row>
     <row r="1976" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1976" s="7" t="s">
@@ -16484,14 +16682,14 @@
         <v>2.1</v>
       </c>
       <c r="D1980" s="10"/>
-      <c r="E1980" s="47" t="s">
+      <c r="E1980" s="48" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="1981" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1981" s="9"/>
       <c r="D1981" s="10"/>
-      <c r="E1981" s="47"/>
+      <c r="E1981" s="48"/>
     </row>
     <row r="1982" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1982" s="9">
@@ -16512,41 +16710,41 @@
       <c r="E1983" s="17"/>
     </row>
     <row r="1985" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1985" s="49" t="e" vm="44">
+      <c r="C1985" s="44" t="e" vm="44">
         <v>#VALUE!</v>
       </c>
-      <c r="D1985" s="49"/>
-      <c r="E1985" s="49"/>
+      <c r="D1985" s="44"/>
+      <c r="E1985" s="44"/>
     </row>
     <row r="1986" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1986" s="49"/>
-      <c r="D1986" s="49"/>
-      <c r="E1986" s="49"/>
+      <c r="C1986" s="44"/>
+      <c r="D1986" s="44"/>
+      <c r="E1986" s="44"/>
     </row>
     <row r="1987" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1987" s="49"/>
-      <c r="D1987" s="49"/>
-      <c r="E1987" s="49"/>
+      <c r="C1987" s="44"/>
+      <c r="D1987" s="44"/>
+      <c r="E1987" s="44"/>
     </row>
     <row r="1988" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1988" s="49"/>
-      <c r="D1988" s="49"/>
-      <c r="E1988" s="49"/>
+      <c r="C1988" s="44"/>
+      <c r="D1988" s="44"/>
+      <c r="E1988" s="44"/>
     </row>
     <row r="1989" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1989" s="49"/>
-      <c r="D1989" s="49"/>
-      <c r="E1989" s="49"/>
+      <c r="C1989" s="44"/>
+      <c r="D1989" s="44"/>
+      <c r="E1989" s="44"/>
     </row>
     <row r="1990" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1990" s="49"/>
-      <c r="D1990" s="49"/>
-      <c r="E1990" s="49"/>
+      <c r="C1990" s="44"/>
+      <c r="D1990" s="44"/>
+      <c r="E1990" s="44"/>
     </row>
     <row r="1991" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1991" s="49"/>
-      <c r="D1991" s="49"/>
-      <c r="E1991" s="49"/>
+      <c r="C1991" s="44"/>
+      <c r="D1991" s="44"/>
+      <c r="E1991" s="44"/>
     </row>
     <row r="2021" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2021" s="1" t="s">
@@ -16561,10 +16759,10 @@
     </row>
     <row r="2022" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2022" s="21"/>
-      <c r="D2022" s="44" t="s">
+      <c r="D2022" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="E2022" s="45"/>
+      <c r="E2022" s="46"/>
     </row>
     <row r="2023" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2023" s="7" t="s">
@@ -16613,14 +16811,14 @@
         <v>2.1</v>
       </c>
       <c r="D2027" s="10"/>
-      <c r="E2027" s="47" t="s">
+      <c r="E2027" s="48" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="2028" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2028" s="9"/>
       <c r="D2028" s="10"/>
-      <c r="E2028" s="47"/>
+      <c r="E2028" s="48"/>
     </row>
     <row r="2029" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2029" s="9">
@@ -16643,20 +16841,20 @@
       </c>
     </row>
     <row r="2032" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2032" s="46" t="s">
+      <c r="B2032" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C2032" s="46"/>
-      <c r="D2032" s="46"/>
-      <c r="E2032" s="46"/>
+      <c r="C2032" s="47"/>
+      <c r="D2032" s="47"/>
+      <c r="E2032" s="47"/>
     </row>
     <row r="2033" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2033" s="48" t="s">
+      <c r="B2033" s="50" t="s">
         <v>60</v>
       </c>
-      <c r="C2033" s="48"/>
-      <c r="D2033" s="48"/>
-      <c r="E2033" s="48"/>
+      <c r="C2033" s="50"/>
+      <c r="D2033" s="50"/>
+      <c r="E2033" s="50"/>
     </row>
     <row r="2035" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2035" s="43" t="e" vm="45">
@@ -16768,11 +16966,11 @@
       <c r="E2056" s="43"/>
     </row>
     <row r="2057" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2057" s="48" t="s">
+      <c r="C2057" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="D2057" s="48"/>
-      <c r="E2057" s="48"/>
+      <c r="D2057" s="50"/>
+      <c r="E2057" s="50"/>
     </row>
     <row r="2068" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2068" s="1" t="s">
@@ -16787,10 +16985,10 @@
     </row>
     <row r="2069" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2069" s="21"/>
-      <c r="D2069" s="44" t="s">
+      <c r="D2069" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="E2069" s="45"/>
+      <c r="E2069" s="46"/>
     </row>
     <row r="2070" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2070" s="7" t="s">
@@ -16985,10 +17183,10 @@
     </row>
     <row r="2116" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2116" s="21"/>
-      <c r="D2116" s="44" t="s">
+      <c r="D2116" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="E2116" s="45"/>
+      <c r="E2116" s="46"/>
     </row>
     <row r="2117" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2117" s="7" t="s">
@@ -17107,12 +17305,12 @@
       <c r="E2128" s="14"/>
     </row>
     <row r="2129" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2129" s="46" t="s">
+      <c r="B2129" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C2129" s="46"/>
-      <c r="D2129" s="46"/>
-      <c r="E2129" s="46"/>
+      <c r="C2129" s="47"/>
+      <c r="D2129" s="47"/>
+      <c r="E2129" s="47"/>
     </row>
     <row r="2131" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2131" s="43" t="e" vm="47">
@@ -17184,10 +17382,10 @@
     </row>
     <row r="2163" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2163" s="21"/>
-      <c r="D2163" s="44" t="s">
+      <c r="D2163" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="E2163" s="45"/>
+      <c r="E2163" s="46"/>
     </row>
     <row r="2164" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2164" s="7" t="s">
@@ -17294,14 +17492,14 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D2174" s="10"/>
-      <c r="E2174" s="47" t="s">
+      <c r="E2174" s="48" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="2175" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2175" s="9"/>
       <c r="D2175" s="10"/>
-      <c r="E2175" s="47"/>
+      <c r="E2175" s="48"/>
     </row>
     <row r="2176" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2176" s="40">
@@ -17424,10 +17622,10 @@
     </row>
     <row r="2210" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2210" s="21"/>
-      <c r="D2210" s="44" t="s">
+      <c r="D2210" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="E2210" s="45"/>
+      <c r="E2210" s="46"/>
     </row>
     <row r="2211" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2211" s="7" t="s">
@@ -17534,19 +17732,19 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D2221" s="10"/>
-      <c r="E2221" s="47" t="s">
+      <c r="E2221" s="48" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="2222" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2222" s="9"/>
       <c r="D2222" s="10"/>
-      <c r="E2222" s="47"/>
+      <c r="E2222" s="48"/>
     </row>
     <row r="2223" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2223" s="9"/>
       <c r="D2223" s="10"/>
-      <c r="E2223" s="47"/>
+      <c r="E2223" s="48"/>
     </row>
     <row r="2224" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2224" s="40">
@@ -17592,12 +17790,12 @@
       <c r="E2228" s="14"/>
     </row>
     <row r="2229" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2229" s="46" t="s">
+      <c r="B2229" s="47" t="s">
         <v>170</v>
       </c>
-      <c r="C2229" s="46"/>
-      <c r="D2229" s="46"/>
-      <c r="E2229" s="46"/>
+      <c r="C2229" s="47"/>
+      <c r="D2229" s="47"/>
+      <c r="E2229" s="47"/>
     </row>
     <row r="2231" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2231" s="43" t="e" vm="49">
@@ -17684,10 +17882,10 @@
     </row>
     <row r="2257" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2257" s="21"/>
-      <c r="D2257" s="44" t="s">
+      <c r="D2257" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="E2257" s="45"/>
+      <c r="E2257" s="46"/>
     </row>
     <row r="2258" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2258" s="7" t="s">
@@ -17727,14 +17925,14 @@
       <c r="D2261" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E2261" s="47" t="s">
+      <c r="E2261" s="48" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="2262" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2262" s="9"/>
       <c r="D2262" s="10"/>
-      <c r="E2262" s="47"/>
+      <c r="E2262" s="48"/>
     </row>
     <row r="2263" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2263" s="9">
@@ -17759,14 +17957,14 @@
         <v>3.1</v>
       </c>
       <c r="D2265" s="10"/>
-      <c r="E2265" s="47" t="s">
+      <c r="E2265" s="48" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="2266" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2266" s="9"/>
       <c r="D2266" s="10"/>
-      <c r="E2266" s="47"/>
+      <c r="E2266" s="48"/>
     </row>
     <row r="2267" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2267" s="40">
@@ -17958,10 +18156,10 @@
     </row>
     <row r="2304" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2304" s="21"/>
-      <c r="D2304" s="44" t="s">
+      <c r="D2304" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="E2304" s="45"/>
+      <c r="E2304" s="46"/>
     </row>
     <row r="2305" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2305" s="7" t="s">
@@ -18059,14 +18257,14 @@
       <c r="D2314" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E2314" s="47" t="s">
+      <c r="E2314" s="48" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="2315" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2315" s="9"/>
       <c r="D2315" s="10"/>
-      <c r="E2315" s="47"/>
+      <c r="E2315" s="48"/>
     </row>
     <row r="2316" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2316" s="29">
@@ -18118,12 +18316,12 @@
       </c>
     </row>
     <row r="2322" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2322" s="46" t="s">
+      <c r="B2322" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C2322" s="46"/>
-      <c r="D2322" s="46"/>
-      <c r="E2322" s="46"/>
+      <c r="C2322" s="47"/>
+      <c r="D2322" s="47"/>
+      <c r="E2322" s="47"/>
     </row>
     <row r="2324" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2324" s="43" t="e" vm="53">
@@ -18210,10 +18408,10 @@
     </row>
     <row r="2351" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2351" s="21"/>
-      <c r="D2351" s="44" t="s">
+      <c r="D2351" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E2351" s="45"/>
+      <c r="E2351" s="46"/>
     </row>
     <row r="2352" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2352" s="7" t="s">
@@ -18421,10 +18619,10 @@
     </row>
     <row r="2398" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2398" s="21"/>
-      <c r="D2398" s="44" t="s">
+      <c r="D2398" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="E2398" s="45"/>
+      <c r="E2398" s="46"/>
     </row>
     <row r="2399" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2399" s="7" t="s">
@@ -18569,19 +18767,19 @@
         <v>7.1</v>
       </c>
       <c r="D2413" s="10"/>
-      <c r="E2413" s="47" t="s">
+      <c r="E2413" s="48" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="2414" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2414" s="9"/>
       <c r="D2414" s="10"/>
-      <c r="E2414" s="47"/>
+      <c r="E2414" s="48"/>
     </row>
     <row r="2415" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2415" s="9"/>
       <c r="D2415" s="10"/>
-      <c r="E2415" s="47"/>
+      <c r="E2415" s="48"/>
     </row>
     <row r="2416" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2416" s="40">
@@ -18622,12 +18820,12 @@
       </c>
     </row>
     <row r="2421" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2421" s="46" t="s">
+      <c r="B2421" s="47" t="s">
         <v>170</v>
       </c>
-      <c r="C2421" s="46"/>
-      <c r="D2421" s="46"/>
-      <c r="E2421" s="46"/>
+      <c r="C2421" s="47"/>
+      <c r="D2421" s="47"/>
+      <c r="E2421" s="47"/>
     </row>
     <row r="2423" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2423" s="43" t="e" vm="54">
@@ -18729,10 +18927,10 @@
     </row>
     <row r="2445" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2445" s="21"/>
-      <c r="D2445" s="44" t="s">
+      <c r="D2445" s="45" t="s">
         <v>245</v>
       </c>
-      <c r="E2445" s="45"/>
+      <c r="E2445" s="46"/>
     </row>
     <row r="2446" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2446" s="7" t="s">
@@ -18911,10 +19109,10 @@
     </row>
     <row r="2492" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2492" s="21"/>
-      <c r="D2492" s="44" t="s">
+      <c r="D2492" s="45" t="s">
         <v>245</v>
       </c>
-      <c r="E2492" s="45"/>
+      <c r="E2492" s="46"/>
     </row>
     <row r="2493" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2493" s="7" t="s">
@@ -19033,12 +19231,12 @@
       <c r="E2504" s="14"/>
     </row>
     <row r="2505" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2505" s="46" t="s">
+      <c r="B2505" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C2505" s="46"/>
-      <c r="D2505" s="46"/>
-      <c r="E2505" s="46"/>
+      <c r="C2505" s="47"/>
+      <c r="D2505" s="47"/>
+      <c r="E2505" s="47"/>
     </row>
     <row r="2507" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2507" s="43" t="e" vm="56">
@@ -19110,10 +19308,10 @@
     </row>
     <row r="2539" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2539" s="21"/>
-      <c r="D2539" s="44" t="s">
+      <c r="D2539" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="E2539" s="45"/>
+      <c r="E2539" s="46"/>
     </row>
     <row r="2540" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2540" s="7" t="s">
@@ -19220,14 +19418,14 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D2550" s="10"/>
-      <c r="E2550" s="47" t="s">
+      <c r="E2550" s="48" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="2551" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2551" s="9"/>
       <c r="D2551" s="10"/>
-      <c r="E2551" s="47"/>
+      <c r="E2551" s="48"/>
     </row>
     <row r="2552" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2552" s="40">
@@ -19350,10 +19548,10 @@
     </row>
     <row r="2586" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2586" s="21"/>
-      <c r="D2586" s="44" t="s">
+      <c r="D2586" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="E2586" s="45"/>
+      <c r="E2586" s="46"/>
     </row>
     <row r="2587" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2587" s="7" t="s">
@@ -19460,19 +19658,19 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D2597" s="10"/>
-      <c r="E2597" s="47" t="s">
+      <c r="E2597" s="48" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="2598" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2598" s="9"/>
       <c r="D2598" s="10"/>
-      <c r="E2598" s="47"/>
+      <c r="E2598" s="48"/>
     </row>
     <row r="2599" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2599" s="9"/>
       <c r="D2599" s="10"/>
-      <c r="E2599" s="47"/>
+      <c r="E2599" s="48"/>
     </row>
     <row r="2600" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2600" s="40">
@@ -19518,12 +19716,12 @@
       <c r="E2604" s="14"/>
     </row>
     <row r="2605" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2605" s="46" t="s">
+      <c r="B2605" s="47" t="s">
         <v>170</v>
       </c>
-      <c r="C2605" s="46"/>
-      <c r="D2605" s="46"/>
-      <c r="E2605" s="46"/>
+      <c r="C2605" s="47"/>
+      <c r="D2605" s="47"/>
+      <c r="E2605" s="47"/>
     </row>
     <row r="2607" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2607" s="43" t="e" vm="58">
@@ -19610,10 +19808,10 @@
     </row>
     <row r="2633" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2633" s="21"/>
-      <c r="D2633" s="44" t="s">
+      <c r="D2633" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E2633" s="45"/>
+      <c r="E2633" s="46"/>
     </row>
     <row r="2634" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2634" s="7" t="s">
@@ -19739,10 +19937,10 @@
     </row>
     <row r="2680" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2680" s="21"/>
-      <c r="D2680" s="44" t="s">
+      <c r="D2680" s="45" t="s">
         <v>247</v>
       </c>
-      <c r="E2680" s="45"/>
+      <c r="E2680" s="46"/>
     </row>
     <row r="2681" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2681" s="7" t="s">
@@ -19822,14 +20020,14 @@
       <c r="D2688" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E2688" s="47" t="s">
+      <c r="E2688" s="48" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="2689" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2689" s="9"/>
       <c r="D2689" s="10"/>
-      <c r="E2689" s="47"/>
+      <c r="E2689" s="48"/>
     </row>
     <row r="2690" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2690" s="29">
@@ -19881,12 +20079,12 @@
       </c>
     </row>
     <row r="2696" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2696" s="46" t="s">
+      <c r="B2696" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C2696" s="46"/>
-      <c r="D2696" s="46"/>
-      <c r="E2696" s="46"/>
+      <c r="C2696" s="47"/>
+      <c r="D2696" s="47"/>
+      <c r="E2696" s="47"/>
     </row>
     <row r="2698" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2698" s="43" t="e" vm="60">
@@ -19963,10 +20161,10 @@
     </row>
     <row r="2727" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2727" s="21"/>
-      <c r="D2727" s="44" t="s">
+      <c r="D2727" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E2727" s="45"/>
+      <c r="E2727" s="46"/>
     </row>
     <row r="2728" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2728" s="7" t="s">
@@ -20085,10 +20283,10 @@
     </row>
     <row r="2774" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2774" s="21"/>
-      <c r="D2774" s="44" t="s">
+      <c r="D2774" s="45" t="s">
         <v>248</v>
       </c>
-      <c r="E2774" s="45"/>
+      <c r="E2774" s="46"/>
     </row>
     <row r="2775" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2775" s="7" t="s">
@@ -20215,19 +20413,19 @@
         <v>6.1</v>
       </c>
       <c r="D2787" s="10"/>
-      <c r="E2787" s="47" t="s">
+      <c r="E2787" s="48" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="2788" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2788" s="9"/>
       <c r="D2788" s="10"/>
-      <c r="E2788" s="47"/>
+      <c r="E2788" s="48"/>
     </row>
     <row r="2789" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2789" s="9"/>
       <c r="D2789" s="10"/>
-      <c r="E2789" s="47"/>
+      <c r="E2789" s="48"/>
     </row>
     <row r="2790" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2790" s="40">
@@ -20268,12 +20466,12 @@
       </c>
     </row>
     <row r="2795" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2795" s="46" t="s">
+      <c r="B2795" s="47" t="s">
         <v>170</v>
       </c>
-      <c r="C2795" s="46"/>
-      <c r="D2795" s="46"/>
-      <c r="E2795" s="46"/>
+      <c r="C2795" s="47"/>
+      <c r="D2795" s="47"/>
+      <c r="E2795" s="47"/>
     </row>
     <row r="2797" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2797" s="43" t="e" vm="62">
@@ -20365,10 +20563,10 @@
     </row>
     <row r="2821" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2821" s="21"/>
-      <c r="D2821" s="44" t="s">
+      <c r="D2821" s="45" t="s">
         <v>244</v>
       </c>
-      <c r="E2821" s="45"/>
+      <c r="E2821" s="46"/>
     </row>
     <row r="2822" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2822" s="7" t="s">
@@ -20448,14 +20646,14 @@
       <c r="D2829" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E2829" s="47" t="s">
+      <c r="E2829" s="48" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="2830" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2830" s="9"/>
       <c r="D2830" s="10"/>
-      <c r="E2830" s="47"/>
+      <c r="E2830" s="48"/>
     </row>
     <row r="2831" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2831" s="29">
@@ -20572,10 +20770,10 @@
     </row>
     <row r="2868" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2868" s="21"/>
-      <c r="D2868" s="44" t="s">
+      <c r="D2868" s="45" t="s">
         <v>244</v>
       </c>
-      <c r="E2868" s="45"/>
+      <c r="E2868" s="46"/>
     </row>
     <row r="2869" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2869" s="7" t="s">
@@ -20655,14 +20853,14 @@
       <c r="D2876" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E2876" s="47" t="s">
+      <c r="E2876" s="48" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="2877" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2877" s="9"/>
       <c r="D2877" s="10"/>
-      <c r="E2877" s="47"/>
+      <c r="E2877" s="48"/>
     </row>
     <row r="2878" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2878" s="29">
@@ -20719,12 +20917,12 @@
       <c r="E2883" s="14"/>
     </row>
     <row r="2884" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2884" s="46" t="s">
+      <c r="B2884" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C2884" s="46"/>
-      <c r="D2884" s="46"/>
-      <c r="E2884" s="46"/>
+      <c r="C2884" s="47"/>
+      <c r="D2884" s="47"/>
+      <c r="E2884" s="47"/>
     </row>
     <row r="2886" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2886" s="43" t="e" vm="64">
@@ -20801,10 +20999,10 @@
     </row>
     <row r="2915" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2915" s="21"/>
-      <c r="D2915" s="44" t="s">
+      <c r="D2915" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="E2915" s="45"/>
+      <c r="E2915" s="46"/>
     </row>
     <row r="2916" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2916" s="7" t="s">
@@ -20931,14 +21129,14 @@
         <v>6.1</v>
       </c>
       <c r="D2928" s="10"/>
-      <c r="E2928" s="47" t="s">
+      <c r="E2928" s="48" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="2929" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2929" s="9"/>
       <c r="D2929" s="10"/>
-      <c r="E2929" s="47"/>
+      <c r="E2929" s="48"/>
     </row>
     <row r="2930" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2930" s="40">
@@ -21066,10 +21264,10 @@
     </row>
     <row r="2962" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2962" s="21"/>
-      <c r="D2962" s="44" t="s">
+      <c r="D2962" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="E2962" s="45"/>
+      <c r="E2962" s="46"/>
     </row>
     <row r="2963" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2963" s="7" t="s">
@@ -21196,19 +21394,19 @@
         <v>6.1</v>
       </c>
       <c r="D2975" s="10"/>
-      <c r="E2975" s="47" t="s">
+      <c r="E2975" s="48" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="2976" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2976" s="9"/>
       <c r="D2976" s="10"/>
-      <c r="E2976" s="47"/>
+      <c r="E2976" s="48"/>
     </row>
     <row r="2977" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2977" s="9"/>
       <c r="D2977" s="10"/>
-      <c r="E2977" s="47"/>
+      <c r="E2977" s="48"/>
     </row>
     <row r="2978" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2978" s="40">
@@ -21254,12 +21452,12 @@
       <c r="E2982" s="14"/>
     </row>
     <row r="2983" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2983" s="46" t="s">
+      <c r="B2983" s="47" t="s">
         <v>170</v>
       </c>
-      <c r="C2983" s="46"/>
-      <c r="D2983" s="46"/>
-      <c r="E2983" s="46"/>
+      <c r="C2983" s="47"/>
+      <c r="D2983" s="47"/>
+      <c r="E2983" s="47"/>
     </row>
     <row r="2985" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2985" s="43" t="e" vm="66">
@@ -21351,10 +21549,10 @@
     </row>
     <row r="3009" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3009" s="21"/>
-      <c r="D3009" s="44" t="s">
+      <c r="D3009" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E3009" s="45"/>
+      <c r="E3009" s="46"/>
     </row>
     <row r="3010" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3010" s="7" t="s">
@@ -21439,14 +21637,14 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D3018" s="10"/>
-      <c r="E3018" s="47" t="s">
+      <c r="E3018" s="48" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="3019" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3019" s="9"/>
       <c r="D3019" s="10"/>
-      <c r="E3019" s="47"/>
+      <c r="E3019" s="48"/>
     </row>
     <row r="3020" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3020" s="9">
@@ -21591,10 +21789,10 @@
     </row>
     <row r="3056" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3056" s="21"/>
-      <c r="D3056" s="44" t="s">
+      <c r="D3056" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="E3056" s="45"/>
+      <c r="E3056" s="46"/>
     </row>
     <row r="3057" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3057" s="7" t="s">
@@ -21747,12 +21945,12 @@
       <c r="E3072" s="14"/>
     </row>
     <row r="3073" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3073" s="46" t="s">
+      <c r="B3073" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C3073" s="46"/>
-      <c r="D3073" s="46"/>
-      <c r="E3073" s="46"/>
+      <c r="C3073" s="47"/>
+      <c r="D3073" s="47"/>
+      <c r="E3073" s="47"/>
     </row>
     <row r="3074" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3074" s="24"/>
@@ -21844,10 +22042,10 @@
     </row>
     <row r="3103" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3103" s="21"/>
-      <c r="D3103" s="44" t="s">
+      <c r="D3103" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E3103" s="45"/>
+      <c r="E3103" s="46"/>
     </row>
     <row r="3104" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3104" s="7" t="s">
@@ -22055,10 +22253,10 @@
     </row>
     <row r="3150" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3150" s="21"/>
-      <c r="D3150" s="44" t="s">
+      <c r="D3150" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="E3150" s="45"/>
+      <c r="E3150" s="46"/>
     </row>
     <row r="3151" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3151" s="7" t="s">
@@ -22201,14 +22399,14 @@
         <v>7.1</v>
       </c>
       <c r="D3165" s="10"/>
-      <c r="E3165" s="47" t="s">
+      <c r="E3165" s="48" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="3166" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3166" s="9"/>
       <c r="D3166" s="10"/>
-      <c r="E3166" s="47"/>
+      <c r="E3166" s="48"/>
     </row>
     <row r="3167" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3167" s="40">
@@ -22249,12 +22447,12 @@
       </c>
     </row>
     <row r="3172" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3172" s="46" t="s">
+      <c r="B3172" s="47" t="s">
         <v>170</v>
       </c>
-      <c r="C3172" s="46"/>
-      <c r="D3172" s="46"/>
-      <c r="E3172" s="46"/>
+      <c r="C3172" s="47"/>
+      <c r="D3172" s="47"/>
+      <c r="E3172" s="47"/>
     </row>
     <row r="3174" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3174" s="43" t="e" vm="69">
@@ -22356,10 +22554,10 @@
     </row>
     <row r="3197" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3197" s="21"/>
-      <c r="D3197" s="44" t="s">
+      <c r="D3197" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="E3197" s="45"/>
+      <c r="E3197" s="46"/>
     </row>
     <row r="3198" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3198" s="7" t="s">
@@ -22508,10 +22706,10 @@
     </row>
     <row r="3244" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3244" s="21"/>
-      <c r="D3244" s="44" t="s">
+      <c r="D3244" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="E3244" s="45"/>
+      <c r="E3244" s="46"/>
     </row>
     <row r="3245" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3245" s="7" t="s">
@@ -22605,12 +22803,12 @@
       </c>
     </row>
     <row r="3255" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3255" s="46" t="s">
+      <c r="B3255" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C3255" s="46"/>
-      <c r="D3255" s="46"/>
-      <c r="E3255" s="46"/>
+      <c r="C3255" s="47"/>
+      <c r="D3255" s="47"/>
+      <c r="E3255" s="47"/>
     </row>
     <row r="3257" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3257" s="43" t="e" vm="71">
@@ -22672,10 +22870,10 @@
     </row>
     <row r="3291" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3291" s="21"/>
-      <c r="D3291" s="44" t="s">
+      <c r="D3291" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="E3291" s="45"/>
+      <c r="E3291" s="46"/>
     </row>
     <row r="3292" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3292" s="7" t="s">
@@ -22877,10 +23075,10 @@
     </row>
     <row r="3338" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3338" s="21"/>
-      <c r="D3338" s="44" t="s">
+      <c r="D3338" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="E3338" s="45"/>
+      <c r="E3338" s="46"/>
     </row>
     <row r="3339" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3339" s="7" t="s">
@@ -22969,14 +23167,14 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D3347" s="10"/>
-      <c r="E3347" s="47" t="s">
+      <c r="E3347" s="48" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="3348" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3348" s="9"/>
       <c r="D3348" s="10"/>
-      <c r="E3348" s="47"/>
+      <c r="E3348" s="48"/>
     </row>
     <row r="3349" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3349" s="40">
@@ -23017,12 +23215,12 @@
       </c>
     </row>
     <row r="3354" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3354" s="46" t="s">
+      <c r="B3354" s="47" t="s">
         <v>170</v>
       </c>
-      <c r="C3354" s="46"/>
-      <c r="D3354" s="46"/>
-      <c r="E3354" s="46"/>
+      <c r="C3354" s="47"/>
+      <c r="D3354" s="47"/>
+      <c r="E3354" s="47"/>
     </row>
     <row r="3356" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3356" s="43" t="e" vm="73">
@@ -23099,10 +23297,10 @@
     </row>
     <row r="3385" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3385" s="21"/>
-      <c r="D3385" s="44" t="s">
+      <c r="D3385" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E3385" s="45"/>
+      <c r="E3385" s="46"/>
     </row>
     <row r="3386" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3386" s="7" t="s">
@@ -23249,10 +23447,10 @@
     </row>
     <row r="3432" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3432" s="21"/>
-      <c r="D3432" s="44" t="s">
+      <c r="D3432" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="E3432" s="45"/>
+      <c r="E3432" s="46"/>
     </row>
     <row r="3433" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3433" s="7" t="s">
@@ -23326,12 +23524,12 @@
       </c>
     </row>
     <row r="3441" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3441" s="46" t="s">
+      <c r="B3441" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C3441" s="46"/>
-      <c r="D3441" s="46"/>
-      <c r="E3441" s="46"/>
+      <c r="C3441" s="47"/>
+      <c r="D3441" s="47"/>
+      <c r="E3441" s="47"/>
     </row>
     <row r="3443" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3443" s="43" t="e" vm="75">
@@ -23383,10 +23581,10 @@
     </row>
     <row r="3479" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3479" s="21"/>
-      <c r="D3479" s="44" t="s">
+      <c r="D3479" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E3479" s="45"/>
+      <c r="E3479" s="46"/>
     </row>
     <row r="3480" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3480" s="7" t="s">
@@ -23435,14 +23633,14 @@
         <v>2.1</v>
       </c>
       <c r="D3484" s="10"/>
-      <c r="E3484" s="47" t="s">
+      <c r="E3484" s="48" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="3485" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3485" s="9"/>
       <c r="D3485" s="10"/>
-      <c r="E3485" s="47"/>
+      <c r="E3485" s="48"/>
     </row>
     <row r="3486" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3486" s="9">
@@ -23465,12 +23663,12 @@
       </c>
     </row>
     <row r="3489" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3489" s="46" t="s">
+      <c r="B3489" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C3489" s="46"/>
-      <c r="D3489" s="46"/>
-      <c r="E3489" s="46"/>
+      <c r="C3489" s="47"/>
+      <c r="D3489" s="47"/>
+      <c r="E3489" s="47"/>
     </row>
     <row r="3491" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3491" s="43" t="e" vm="76">
@@ -23522,10 +23720,10 @@
     </row>
     <row r="3526" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3526" s="21"/>
-      <c r="D3526" s="44" t="s">
+      <c r="D3526" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="E3526" s="45"/>
+      <c r="E3526" s="46"/>
     </row>
     <row r="3527" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3527" s="7" t="s">
@@ -23574,14 +23772,14 @@
         <v>2.1</v>
       </c>
       <c r="D3531" s="10"/>
-      <c r="E3531" s="47" t="s">
+      <c r="E3531" s="48" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="3532" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3532" s="9"/>
       <c r="D3532" s="10"/>
-      <c r="E3532" s="47"/>
+      <c r="E3532" s="48"/>
     </row>
     <row r="3533" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3533" s="9">
@@ -23651,10 +23849,10 @@
     </row>
     <row r="3573" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3573" s="21"/>
-      <c r="D3573" s="44" t="s">
+      <c r="D3573" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="E3573" s="45"/>
+      <c r="E3573" s="46"/>
     </row>
     <row r="3574" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3574" s="7" t="s">
@@ -23805,10 +24003,10 @@
     </row>
     <row r="3620" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3620" s="21"/>
-      <c r="D3620" s="44" t="s">
+      <c r="D3620" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="E3620" s="45"/>
+      <c r="E3620" s="46"/>
     </row>
     <row r="3621" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3621" s="7" t="s">
@@ -23922,12 +24120,12 @@
       </c>
     </row>
     <row r="3633" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3633" s="46" t="s">
+      <c r="B3633" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C3633" s="46"/>
-      <c r="D3633" s="46"/>
-      <c r="E3633" s="46"/>
+      <c r="C3633" s="47"/>
+      <c r="D3633" s="47"/>
+      <c r="E3633" s="47"/>
     </row>
     <row r="3635" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3635" s="43" t="e" vm="79">
@@ -23994,10 +24192,10 @@
     </row>
     <row r="3667" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3667" s="21"/>
-      <c r="D3667" s="44" t="s">
+      <c r="D3667" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="E3667" s="45"/>
+      <c r="E3667" s="46"/>
     </row>
     <row r="3668" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3668" s="7" t="s">
@@ -24231,10 +24429,10 @@
     </row>
     <row r="3714" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3714" s="21"/>
-      <c r="D3714" s="44" t="s">
+      <c r="D3714" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="E3714" s="45"/>
+      <c r="E3714" s="46"/>
     </row>
     <row r="3715" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3715" s="7" t="s">
@@ -24343,14 +24541,14 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D3725" s="10"/>
-      <c r="E3725" s="47" t="s">
+      <c r="E3725" s="48" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="3726" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3726" s="9"/>
       <c r="D3726" s="10"/>
-      <c r="E3726" s="47"/>
+      <c r="E3726" s="48"/>
     </row>
     <row r="3727" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3727" s="40">
@@ -24396,12 +24594,12 @@
       <c r="E3731" s="14"/>
     </row>
     <row r="3732" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3732" s="46" t="s">
+      <c r="B3732" s="47" t="s">
         <v>170</v>
       </c>
-      <c r="C3732" s="46"/>
-      <c r="D3732" s="46"/>
-      <c r="E3732" s="46"/>
+      <c r="C3732" s="47"/>
+      <c r="D3732" s="47"/>
+      <c r="E3732" s="47"/>
     </row>
     <row r="3734" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3734" s="43" t="e" vm="81">
@@ -24488,10 +24686,10 @@
     </row>
     <row r="3761" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3761" s="21"/>
-      <c r="D3761" s="44" t="s">
+      <c r="D3761" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="E3761" s="45"/>
+      <c r="E3761" s="46"/>
     </row>
     <row r="3762" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3762" s="7" t="s">
@@ -24531,14 +24729,14 @@
       <c r="D3765" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E3765" s="47" t="s">
+      <c r="E3765" s="48" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="3766" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3766" s="9"/>
       <c r="D3766" s="10"/>
-      <c r="E3766" s="47"/>
+      <c r="E3766" s="48"/>
     </row>
     <row r="3767" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3767" s="9">
@@ -24563,14 +24761,14 @@
         <v>3.1</v>
       </c>
       <c r="D3769" s="10"/>
-      <c r="E3769" s="47" t="s">
+      <c r="E3769" s="48" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="3770" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3770" s="9"/>
       <c r="D3770" s="10"/>
-      <c r="E3770" s="47"/>
+      <c r="E3770" s="48"/>
     </row>
     <row r="3771" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3771" s="40">
@@ -24762,10 +24960,10 @@
     </row>
     <row r="3808" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3808" s="21"/>
-      <c r="D3808" s="44" t="s">
+      <c r="D3808" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="E3808" s="45"/>
+      <c r="E3808" s="46"/>
     </row>
     <row r="3809" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3809" s="7" t="s">
@@ -24863,14 +25061,14 @@
       <c r="D3818" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E3818" s="47" t="s">
+      <c r="E3818" s="48" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="3819" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3819" s="9"/>
       <c r="D3819" s="10"/>
-      <c r="E3819" s="47"/>
+      <c r="E3819" s="48"/>
     </row>
     <row r="3820" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3820" s="29">
@@ -24922,12 +25120,12 @@
       </c>
     </row>
     <row r="3826" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3826" s="46" t="s">
+      <c r="B3826" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C3826" s="46"/>
-      <c r="D3826" s="46"/>
-      <c r="E3826" s="46"/>
+      <c r="C3826" s="47"/>
+      <c r="D3826" s="47"/>
+      <c r="E3826" s="47"/>
     </row>
     <row r="3828" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3828" s="43" t="e" vm="85">
@@ -25004,10 +25202,10 @@
     </row>
     <row r="3855" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3855" s="21"/>
-      <c r="D3855" s="44" t="s">
+      <c r="D3855" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E3855" s="45"/>
+      <c r="E3855" s="46"/>
     </row>
     <row r="3856" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3856" s="7" t="s">
@@ -25215,10 +25413,10 @@
     </row>
     <row r="3902" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3902" s="21"/>
-      <c r="D3902" s="44" t="s">
+      <c r="D3902" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="E3902" s="45"/>
+      <c r="E3902" s="46"/>
     </row>
     <row r="3903" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3903" s="7" t="s">
@@ -25365,14 +25563,14 @@
         <v>7.1</v>
       </c>
       <c r="D3917" s="10"/>
-      <c r="E3917" s="47" t="s">
+      <c r="E3917" s="48" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="3918" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3918" s="9"/>
       <c r="D3918" s="10"/>
-      <c r="E3918" s="47"/>
+      <c r="E3918" s="48"/>
     </row>
     <row r="3919" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3919" s="40">
@@ -25413,12 +25611,12 @@
       </c>
     </row>
     <row r="3924" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3924" s="46" t="s">
+      <c r="B3924" s="47" t="s">
         <v>170</v>
       </c>
-      <c r="C3924" s="46"/>
-      <c r="D3924" s="46"/>
-      <c r="E3924" s="46"/>
+      <c r="C3924" s="47"/>
+      <c r="D3924" s="47"/>
+      <c r="E3924" s="47"/>
     </row>
     <row r="3926" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3926" s="43" t="e" vm="86">
@@ -25520,10 +25718,10 @@
     </row>
     <row r="3949" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3949" s="21"/>
-      <c r="D3949" s="44" t="s">
+      <c r="D3949" s="45" t="s">
         <v>245</v>
       </c>
-      <c r="E3949" s="45"/>
+      <c r="E3949" s="46"/>
     </row>
     <row r="3950" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3950" s="7" t="s">
@@ -25702,10 +25900,10 @@
     </row>
     <row r="3996" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3996" s="21"/>
-      <c r="D3996" s="44" t="s">
+      <c r="D3996" s="45" t="s">
         <v>245</v>
       </c>
-      <c r="E3996" s="45"/>
+      <c r="E3996" s="46"/>
     </row>
     <row r="3997" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3997" s="7" t="s">
@@ -25824,12 +26022,12 @@
       <c r="E4008" s="14"/>
     </row>
     <row r="4009" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4009" s="46" t="s">
+      <c r="B4009" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C4009" s="46"/>
-      <c r="D4009" s="46"/>
-      <c r="E4009" s="46"/>
+      <c r="C4009" s="47"/>
+      <c r="D4009" s="47"/>
+      <c r="E4009" s="47"/>
     </row>
     <row r="4011" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4011" s="43" t="e" vm="88">
@@ -25901,10 +26099,10 @@
     </row>
     <row r="4043" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4043" s="21"/>
-      <c r="D4043" s="44" t="s">
+      <c r="D4043" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="E4043" s="45"/>
+      <c r="E4043" s="46"/>
     </row>
     <row r="4044" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4044" s="7" t="s">
@@ -26138,10 +26336,10 @@
     </row>
     <row r="4090" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4090" s="21"/>
-      <c r="D4090" s="44" t="s">
+      <c r="D4090" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="E4090" s="45"/>
+      <c r="E4090" s="46"/>
     </row>
     <row r="4091" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4091" s="7" t="s">
@@ -26250,14 +26448,14 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D4101" s="10"/>
-      <c r="E4101" s="47" t="s">
+      <c r="E4101" s="48" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="4102" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4102" s="9"/>
       <c r="D4102" s="10"/>
-      <c r="E4102" s="47"/>
+      <c r="E4102" s="48"/>
     </row>
     <row r="4103" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4103" s="40">
@@ -26303,12 +26501,12 @@
       <c r="E4107" s="14"/>
     </row>
     <row r="4108" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4108" s="46" t="s">
+      <c r="B4108" s="47" t="s">
         <v>170</v>
       </c>
-      <c r="C4108" s="46"/>
-      <c r="D4108" s="46"/>
-      <c r="E4108" s="46"/>
+      <c r="C4108" s="47"/>
+      <c r="D4108" s="47"/>
+      <c r="E4108" s="47"/>
     </row>
     <row r="4110" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4110" s="43" t="e" vm="90">
@@ -26395,10 +26593,10 @@
     </row>
     <row r="4137" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4137" s="21"/>
-      <c r="D4137" s="44" t="s">
+      <c r="D4137" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E4137" s="45"/>
+      <c r="E4137" s="46"/>
     </row>
     <row r="4138" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4138" s="7" t="s">
@@ -26524,10 +26722,10 @@
     </row>
     <row r="4184" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4184" s="21"/>
-      <c r="D4184" s="44" t="s">
+      <c r="D4184" s="45" t="s">
         <v>247</v>
       </c>
-      <c r="E4184" s="45"/>
+      <c r="E4184" s="46"/>
     </row>
     <row r="4185" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4185" s="7" t="s">
@@ -26607,14 +26805,14 @@
       <c r="D4192" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E4192" s="47" t="s">
+      <c r="E4192" s="48" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="4193" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4193" s="9"/>
       <c r="D4193" s="10"/>
-      <c r="E4193" s="47"/>
+      <c r="E4193" s="48"/>
     </row>
     <row r="4194" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4194" s="29">
@@ -26666,12 +26864,12 @@
       </c>
     </row>
     <row r="4200" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4200" s="46" t="s">
+      <c r="B4200" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C4200" s="46"/>
-      <c r="D4200" s="46"/>
-      <c r="E4200" s="46"/>
+      <c r="C4200" s="47"/>
+      <c r="D4200" s="47"/>
+      <c r="E4200" s="47"/>
     </row>
     <row r="4202" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4202" s="43" t="e" vm="92">
@@ -26748,10 +26946,10 @@
     </row>
     <row r="4231" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4231" s="21"/>
-      <c r="D4231" s="44" t="s">
+      <c r="D4231" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E4231" s="45"/>
+      <c r="E4231" s="46"/>
     </row>
     <row r="4232" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4232" s="7" t="s">
@@ -26870,10 +27068,10 @@
     </row>
     <row r="4278" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4278" s="21"/>
-      <c r="D4278" s="44" t="s">
+      <c r="D4278" s="45" t="s">
         <v>248</v>
       </c>
-      <c r="E4278" s="45"/>
+      <c r="E4278" s="46"/>
     </row>
     <row r="4279" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4279" s="7" t="s">
@@ -27002,14 +27200,14 @@
         <v>6.1</v>
       </c>
       <c r="D4291" s="10"/>
-      <c r="E4291" s="47" t="s">
+      <c r="E4291" s="48" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="4292" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4292" s="9"/>
       <c r="D4292" s="10"/>
-      <c r="E4292" s="47"/>
+      <c r="E4292" s="48"/>
     </row>
     <row r="4293" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4293" s="40">
@@ -27050,12 +27248,12 @@
       </c>
     </row>
     <row r="4298" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4298" s="46" t="s">
+      <c r="B4298" s="47" t="s">
         <v>170</v>
       </c>
-      <c r="C4298" s="46"/>
-      <c r="D4298" s="46"/>
-      <c r="E4298" s="46"/>
+      <c r="C4298" s="47"/>
+      <c r="D4298" s="47"/>
+      <c r="E4298" s="47"/>
     </row>
     <row r="4300" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4300" s="43" t="e" vm="94">
@@ -27147,10 +27345,10 @@
     </row>
     <row r="4325" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4325" s="21"/>
-      <c r="D4325" s="44" t="s">
+      <c r="D4325" s="45" t="s">
         <v>244</v>
       </c>
-      <c r="E4325" s="45"/>
+      <c r="E4325" s="46"/>
     </row>
     <row r="4326" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4326" s="7" t="s">
@@ -27230,14 +27428,14 @@
       <c r="D4333" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E4333" s="47" t="s">
+      <c r="E4333" s="48" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="4334" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4334" s="9"/>
       <c r="D4334" s="10"/>
-      <c r="E4334" s="47"/>
+      <c r="E4334" s="48"/>
     </row>
     <row r="4335" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4335" s="29">
@@ -27359,10 +27557,10 @@
     </row>
     <row r="4372" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4372" s="21"/>
-      <c r="D4372" s="44" t="s">
+      <c r="D4372" s="45" t="s">
         <v>244</v>
       </c>
-      <c r="E4372" s="45"/>
+      <c r="E4372" s="46"/>
     </row>
     <row r="4373" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4373" s="7" t="s">
@@ -27442,14 +27640,14 @@
       <c r="D4380" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E4380" s="47" t="s">
+      <c r="E4380" s="48" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="4381" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4381" s="9"/>
       <c r="D4381" s="10"/>
-      <c r="E4381" s="47"/>
+      <c r="E4381" s="48"/>
     </row>
     <row r="4382" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4382" s="29">
@@ -27506,12 +27704,12 @@
       <c r="E4387" s="14"/>
     </row>
     <row r="4388" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4388" s="46" t="s">
+      <c r="B4388" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C4388" s="46"/>
-      <c r="D4388" s="46"/>
-      <c r="E4388" s="46"/>
+      <c r="C4388" s="47"/>
+      <c r="D4388" s="47"/>
+      <c r="E4388" s="47"/>
     </row>
     <row r="4390" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4390" s="43" t="e" vm="96">
@@ -27588,10 +27786,10 @@
     </row>
     <row r="4419" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4419" s="21"/>
-      <c r="D4419" s="44" t="s">
+      <c r="D4419" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="E4419" s="45"/>
+      <c r="E4419" s="46"/>
     </row>
     <row r="4420" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4420" s="7" t="s">
@@ -27850,10 +28048,10 @@
     </row>
     <row r="4466" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4466" s="21"/>
-      <c r="D4466" s="44" t="s">
+      <c r="D4466" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="E4466" s="45"/>
+      <c r="E4466" s="46"/>
     </row>
     <row r="4467" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4467" s="7" t="s">
@@ -27982,14 +28180,14 @@
         <v>6.1</v>
       </c>
       <c r="D4479" s="10"/>
-      <c r="E4479" s="47" t="s">
+      <c r="E4479" s="48" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="4480" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4480" s="9"/>
       <c r="D4480" s="10"/>
-      <c r="E4480" s="47"/>
+      <c r="E4480" s="48"/>
     </row>
     <row r="4481" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4481" s="40">
@@ -28035,12 +28233,12 @@
       <c r="E4485" s="14"/>
     </row>
     <row r="4486" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4486" s="46" t="s">
+      <c r="B4486" s="47" t="s">
         <v>170</v>
       </c>
-      <c r="C4486" s="46"/>
-      <c r="D4486" s="46"/>
-      <c r="E4486" s="46"/>
+      <c r="C4486" s="47"/>
+      <c r="D4486" s="47"/>
+      <c r="E4486" s="47"/>
     </row>
     <row r="4488" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4488" s="43" t="e" vm="98">
@@ -28132,10 +28330,10 @@
     </row>
     <row r="4513" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4513" s="21"/>
-      <c r="D4513" s="44" t="s">
+      <c r="D4513" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E4513" s="45"/>
+      <c r="E4513" s="46"/>
     </row>
     <row r="4514" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4514" s="7" t="s">
@@ -28279,76 +28477,76 @@
       <c r="E4528" s="17"/>
     </row>
     <row r="4530" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4530" s="49" t="e" vm="99">
+      <c r="C4530" s="44" t="e" vm="99">
         <v>#VALUE!</v>
       </c>
-      <c r="D4530" s="49"/>
-      <c r="E4530" s="49"/>
+      <c r="D4530" s="44"/>
+      <c r="E4530" s="44"/>
     </row>
     <row r="4531" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4531" s="49"/>
-      <c r="D4531" s="49"/>
-      <c r="E4531" s="49"/>
+      <c r="C4531" s="44"/>
+      <c r="D4531" s="44"/>
+      <c r="E4531" s="44"/>
     </row>
     <row r="4532" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4532" s="49"/>
-      <c r="D4532" s="49"/>
-      <c r="E4532" s="49"/>
+      <c r="C4532" s="44"/>
+      <c r="D4532" s="44"/>
+      <c r="E4532" s="44"/>
     </row>
     <row r="4533" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4533" s="49"/>
-      <c r="D4533" s="49"/>
-      <c r="E4533" s="49"/>
+      <c r="C4533" s="44"/>
+      <c r="D4533" s="44"/>
+      <c r="E4533" s="44"/>
     </row>
     <row r="4534" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4534" s="49"/>
-      <c r="D4534" s="49"/>
-      <c r="E4534" s="49"/>
+      <c r="C4534" s="44"/>
+      <c r="D4534" s="44"/>
+      <c r="E4534" s="44"/>
     </row>
     <row r="4535" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4535" s="49"/>
-      <c r="D4535" s="49"/>
-      <c r="E4535" s="49"/>
+      <c r="C4535" s="44"/>
+      <c r="D4535" s="44"/>
+      <c r="E4535" s="44"/>
     </row>
     <row r="4536" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4536" s="49"/>
-      <c r="D4536" s="49"/>
-      <c r="E4536" s="49"/>
+      <c r="C4536" s="44"/>
+      <c r="D4536" s="44"/>
+      <c r="E4536" s="44"/>
     </row>
     <row r="4537" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4537" s="49"/>
-      <c r="D4537" s="49"/>
-      <c r="E4537" s="49"/>
+      <c r="C4537" s="44"/>
+      <c r="D4537" s="44"/>
+      <c r="E4537" s="44"/>
     </row>
     <row r="4538" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4538" s="49"/>
-      <c r="D4538" s="49"/>
-      <c r="E4538" s="49"/>
+      <c r="C4538" s="44"/>
+      <c r="D4538" s="44"/>
+      <c r="E4538" s="44"/>
     </row>
     <row r="4539" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4539" s="49"/>
-      <c r="D4539" s="49"/>
-      <c r="E4539" s="49"/>
+      <c r="C4539" s="44"/>
+      <c r="D4539" s="44"/>
+      <c r="E4539" s="44"/>
     </row>
     <row r="4540" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4540" s="49"/>
-      <c r="D4540" s="49"/>
-      <c r="E4540" s="49"/>
+      <c r="C4540" s="44"/>
+      <c r="D4540" s="44"/>
+      <c r="E4540" s="44"/>
     </row>
     <row r="4541" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4541" s="49"/>
-      <c r="D4541" s="49"/>
-      <c r="E4541" s="49"/>
+      <c r="C4541" s="44"/>
+      <c r="D4541" s="44"/>
+      <c r="E4541" s="44"/>
     </row>
     <row r="4542" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4542" s="49"/>
-      <c r="D4542" s="49"/>
-      <c r="E4542" s="49"/>
+      <c r="C4542" s="44"/>
+      <c r="D4542" s="44"/>
+      <c r="E4542" s="44"/>
     </row>
     <row r="4543" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4543" s="49"/>
-      <c r="D4543" s="49"/>
-      <c r="E4543" s="49"/>
+      <c r="C4543" s="44"/>
+      <c r="D4543" s="44"/>
+      <c r="E4543" s="44"/>
     </row>
     <row r="4559" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4559" s="1" t="s">
@@ -28363,10 +28561,10 @@
     </row>
     <row r="4560" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4560" s="21"/>
-      <c r="D4560" s="44" t="s">
+      <c r="D4560" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="E4560" s="45"/>
+      <c r="E4560" s="46"/>
     </row>
     <row r="4561" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4561" s="7" t="s">
@@ -28554,12 +28752,12 @@
       <c r="E4581" s="14"/>
     </row>
     <row r="4582" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4582" s="46" t="s">
+      <c r="B4582" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C4582" s="46"/>
-      <c r="D4582" s="46"/>
-      <c r="E4582" s="46"/>
+      <c r="C4582" s="47"/>
+      <c r="D4582" s="47"/>
+      <c r="E4582" s="47"/>
     </row>
     <row r="4583" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4583" s="24"/>
@@ -28651,10 +28849,10 @@
     </row>
     <row r="4607" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4607" s="21"/>
-      <c r="D4607" s="44" t="s">
+      <c r="D4607" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E4607" s="45"/>
+      <c r="E4607" s="46"/>
     </row>
     <row r="4608" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4608" s="7" t="s">
@@ -28862,10 +29060,10 @@
     </row>
     <row r="4654" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4654" s="21"/>
-      <c r="D4654" s="44" t="s">
+      <c r="D4654" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="E4654" s="45"/>
+      <c r="E4654" s="46"/>
     </row>
     <row r="4655" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4655" s="7" t="s">
@@ -29070,12 +29268,12 @@
       </c>
     </row>
     <row r="4678" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4678" s="46" t="s">
+      <c r="B4678" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C4678" s="46"/>
-      <c r="D4678" s="46"/>
-      <c r="E4678" s="46"/>
+      <c r="C4678" s="47"/>
+      <c r="D4678" s="47"/>
+      <c r="E4678" s="47"/>
     </row>
     <row r="4680" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4680" s="43" t="e" vm="101">
@@ -29177,10 +29375,10 @@
     </row>
     <row r="4701" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4701" s="21"/>
-      <c r="D4701" s="44" t="s">
+      <c r="D4701" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="E4701" s="45"/>
+      <c r="E4701" s="46"/>
     </row>
     <row r="4702" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4702" s="7" t="s">
@@ -29329,10 +29527,10 @@
     </row>
     <row r="4748" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4748" s="21"/>
-      <c r="D4748" s="44" t="s">
+      <c r="D4748" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="E4748" s="45"/>
+      <c r="E4748" s="46"/>
     </row>
     <row r="4749" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4749" s="7" t="s">
@@ -29461,12 +29659,12 @@
       </c>
     </row>
     <row r="4764" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4764" s="46" t="s">
+      <c r="B4764" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C4764" s="46"/>
-      <c r="D4764" s="46"/>
-      <c r="E4764" s="46"/>
+      <c r="C4764" s="47"/>
+      <c r="D4764" s="47"/>
+      <c r="E4764" s="47"/>
     </row>
     <row r="4766" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4766" s="43" t="e" vm="103">
@@ -29528,10 +29726,10 @@
     </row>
     <row r="4795" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4795" s="21"/>
-      <c r="D4795" s="44" t="s">
+      <c r="D4795" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="E4795" s="45"/>
+      <c r="E4795" s="46"/>
     </row>
     <row r="4796" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4796" s="7" t="s">
@@ -29754,10 +29952,10 @@
     </row>
     <row r="4842" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4842" s="21"/>
-      <c r="D4842" s="44" t="s">
+      <c r="D4842" s="45" t="s">
         <v>243</v>
       </c>
-      <c r="E4842" s="45"/>
+      <c r="E4842" s="46"/>
     </row>
     <row r="4843" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4843" s="7" t="s">
@@ -29908,12 +30106,12 @@
       </c>
     </row>
     <row r="4860" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4860" s="46" t="s">
+      <c r="B4860" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C4860" s="46"/>
-      <c r="D4860" s="46"/>
-      <c r="E4860" s="46"/>
+      <c r="C4860" s="47"/>
+      <c r="D4860" s="47"/>
+      <c r="E4860" s="47"/>
     </row>
     <row r="4862" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4862" s="43" t="e" vm="105">
@@ -30159,180 +30357,612 @@
       <c r="D4912" s="43"/>
       <c r="E4912" s="43"/>
     </row>
+    <row r="4935" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4935" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D4935" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4935" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4936" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4936" s="21"/>
+      <c r="D4936" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4936" s="46"/>
+    </row>
+    <row r="4937" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4937" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4937" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4937" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4938" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4938" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4938" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4938" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4939" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4939" s="9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D4939" s="10"/>
+      <c r="E4939" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4940" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4940" s="40">
+        <v>1.2</v>
+      </c>
+      <c r="D4940" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4940" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4941" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4941" s="9">
+        <v>2.1</v>
+      </c>
+      <c r="D4941" s="10"/>
+      <c r="E4941" s="22" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4942" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4942" s="9"/>
+      <c r="D4942" s="10"/>
+      <c r="E4942" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4943" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4943" s="9"/>
+      <c r="D4943" s="10"/>
+      <c r="E4943" s="22" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="4944" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4944" s="9"/>
+      <c r="D4944" s="10"/>
+      <c r="E4944" s="22" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4945" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4945" s="9"/>
+      <c r="D4945" s="10"/>
+      <c r="E4945" s="22" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="4946" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4946" s="9"/>
+      <c r="D4946" s="10"/>
+      <c r="E4946" s="22" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="4947" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4947" s="9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D4947" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4947" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4948" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4948" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4948" s="16"/>
+      <c r="E4948" s="17" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4950" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4950" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4950" s="47"/>
+      <c r="D4950" s="47"/>
+      <c r="E4950" s="47"/>
+    </row>
+    <row r="4952" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4952" s="43" t="e" vm="107">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D4952" s="43"/>
+      <c r="E4952" s="43"/>
+    </row>
+    <row r="4953" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4953" s="43"/>
+      <c r="D4953" s="43"/>
+      <c r="E4953" s="43"/>
+    </row>
+    <row r="4954" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4954" s="43"/>
+      <c r="D4954" s="43"/>
+      <c r="E4954" s="43"/>
+    </row>
+    <row r="4955" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4955" s="43"/>
+      <c r="D4955" s="43"/>
+      <c r="E4955" s="43"/>
+    </row>
+    <row r="4956" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4956" s="43"/>
+      <c r="D4956" s="43"/>
+      <c r="E4956" s="43"/>
+    </row>
+    <row r="4957" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4957" s="43"/>
+      <c r="D4957" s="43"/>
+      <c r="E4957" s="43"/>
+    </row>
+    <row r="4958" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4958" s="43"/>
+      <c r="D4958" s="43"/>
+      <c r="E4958" s="43"/>
+    </row>
+    <row r="4982" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4982" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="D4982" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4982" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4983" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4983" s="21"/>
+      <c r="D4983" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4983" s="46"/>
+    </row>
+    <row r="4984" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4984" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4984" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4984" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4985" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4985" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4985" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4985" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4986" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4986" s="9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D4986" s="10"/>
+      <c r="E4986" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4987" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4987" s="40">
+        <v>1.2</v>
+      </c>
+      <c r="D4987" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4987" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4988" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4988" s="9">
+        <v>2.1</v>
+      </c>
+      <c r="D4988" s="10"/>
+      <c r="E4988" s="22" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="4989" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4989" s="9"/>
+      <c r="D4989" s="10"/>
+      <c r="E4989" s="22" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="4990" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4990" s="9"/>
+      <c r="D4990" s="10"/>
+      <c r="E4990" s="11" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="4991" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4991" s="9"/>
+      <c r="D4991" s="10"/>
+      <c r="E4991" s="11" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="4992" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4992" s="9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D4992" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4992" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4993" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4993" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4993" s="16"/>
+      <c r="E4993" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4995" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4995" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4995" s="47"/>
+      <c r="D4995" s="47"/>
+      <c r="E4995" s="47"/>
+    </row>
+    <row r="4997" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4997" s="43" t="e" vm="108">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D4997" s="43"/>
+      <c r="E4997" s="43"/>
+    </row>
+    <row r="4998" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4998" s="43"/>
+      <c r="D4998" s="43"/>
+      <c r="E4998" s="43"/>
+    </row>
+    <row r="4999" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4999" s="43"/>
+      <c r="D4999" s="43"/>
+      <c r="E4999" s="43"/>
+    </row>
+    <row r="5000" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5000" s="43"/>
+      <c r="D5000" s="43"/>
+      <c r="E5000" s="43"/>
+    </row>
+    <row r="5001" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5001" s="43"/>
+      <c r="D5001" s="43"/>
+      <c r="E5001" s="43"/>
+    </row>
+    <row r="5002" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5002" s="43"/>
+      <c r="D5002" s="43"/>
+      <c r="E5002" s="43"/>
+    </row>
+    <row r="5003" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5003" s="43"/>
+      <c r="D5003" s="43"/>
+      <c r="E5003" s="43"/>
+    </row>
+    <row r="5029" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5029" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="D5029" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5029" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5030" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5030" s="21"/>
+      <c r="D5030" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5030" s="46"/>
+    </row>
+    <row r="5031" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5031" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5031" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5031" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5032" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5032" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5032" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5032" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5033" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5033" s="9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D5033" s="10"/>
+      <c r="E5033" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5034" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5034" s="40">
+        <v>1.2</v>
+      </c>
+      <c r="D5034" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5034" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5035" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5035" s="9">
+        <v>2.1</v>
+      </c>
+      <c r="D5035" s="10"/>
+      <c r="E5035" s="48" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5036" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5036" s="9"/>
+      <c r="D5036" s="10"/>
+      <c r="E5036" s="48"/>
+    </row>
+    <row r="5037" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5037" s="9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D5037" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5037" s="11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5038" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5038" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5038" s="16"/>
+      <c r="E5038" s="17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5040" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5040" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5040" s="47"/>
+      <c r="D5040" s="47"/>
+      <c r="E5040" s="47"/>
+    </row>
+    <row r="5041" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5041" s="50" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5041" s="50"/>
+      <c r="D5041" s="50"/>
+      <c r="E5041" s="50"/>
+    </row>
+    <row r="5043" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5043" s="43" t="e" vm="12">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D5043" s="43"/>
+      <c r="E5043" s="43"/>
+    </row>
+    <row r="5044" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5044" s="43"/>
+      <c r="D5044" s="43"/>
+      <c r="E5044" s="43"/>
+    </row>
+    <row r="5045" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5045" s="43"/>
+      <c r="D5045" s="43"/>
+      <c r="E5045" s="43"/>
+    </row>
+    <row r="5046" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5046" s="43"/>
+      <c r="D5046" s="43"/>
+      <c r="E5046" s="43"/>
+    </row>
+    <row r="5047" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5047" s="43"/>
+      <c r="D5047" s="43"/>
+      <c r="E5047" s="43"/>
+    </row>
+    <row r="5048" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5048" s="43"/>
+      <c r="D5048" s="43"/>
+      <c r="E5048" s="43"/>
+    </row>
+    <row r="5049" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5049" s="43"/>
+      <c r="D5049" s="43"/>
+      <c r="E5049" s="43"/>
+    </row>
   </sheetData>
-  <mergeCells count="328">
-    <mergeCell ref="C4902:E4912"/>
-    <mergeCell ref="C4530:E4543"/>
-    <mergeCell ref="D4560:E4560"/>
-    <mergeCell ref="B4582:E4582"/>
-    <mergeCell ref="C4584:E4597"/>
-    <mergeCell ref="D4607:E4607"/>
-    <mergeCell ref="C4621:E4637"/>
-    <mergeCell ref="D4419:E4419"/>
-    <mergeCell ref="C4438:E4452"/>
-    <mergeCell ref="D4466:E4466"/>
-    <mergeCell ref="C4488:E4502"/>
-    <mergeCell ref="E4479:E4480"/>
-    <mergeCell ref="B4486:E4486"/>
-    <mergeCell ref="D4513:E4513"/>
-    <mergeCell ref="E4333:E4334"/>
-    <mergeCell ref="C4341:E4352"/>
-    <mergeCell ref="D4372:E4372"/>
-    <mergeCell ref="E4380:E4381"/>
-    <mergeCell ref="C4390:E4401"/>
-    <mergeCell ref="B4388:E4388"/>
-    <mergeCell ref="D4231:E4231"/>
-    <mergeCell ref="C4240:E4246"/>
-    <mergeCell ref="D4278:E4278"/>
-    <mergeCell ref="E4291:E4292"/>
-    <mergeCell ref="B4298:E4298"/>
-    <mergeCell ref="C4300:E4314"/>
-    <mergeCell ref="B4108:E4108"/>
-    <mergeCell ref="D4325:E4325"/>
-    <mergeCell ref="D4090:E4090"/>
-    <mergeCell ref="C4110:E4123"/>
-    <mergeCell ref="E4101:E4102"/>
-    <mergeCell ref="D4137:E4137"/>
-    <mergeCell ref="C4146:E4153"/>
-    <mergeCell ref="D4184:E4184"/>
-    <mergeCell ref="E4192:E4193"/>
-    <mergeCell ref="B4200:E4200"/>
-    <mergeCell ref="C4202:E4213"/>
-    <mergeCell ref="D3949:E3949"/>
-    <mergeCell ref="C3962:E3972"/>
-    <mergeCell ref="D3996:E3996"/>
-    <mergeCell ref="C4011:E4021"/>
-    <mergeCell ref="B4009:E4009"/>
-    <mergeCell ref="D4043:E4043"/>
-    <mergeCell ref="C4060:E4073"/>
-    <mergeCell ref="D3808:E3808"/>
-    <mergeCell ref="E3818:E3819"/>
-    <mergeCell ref="B3826:E3826"/>
-    <mergeCell ref="C3828:E3839"/>
-    <mergeCell ref="D3855:E3855"/>
-    <mergeCell ref="C3869:E3885"/>
-    <mergeCell ref="D3902:E3902"/>
-    <mergeCell ref="E3917:E3918"/>
-    <mergeCell ref="B3924:E3924"/>
-    <mergeCell ref="D3573:E3573"/>
-    <mergeCell ref="D3526:E3526"/>
-    <mergeCell ref="E3531:E3532"/>
-    <mergeCell ref="C3536:E3542"/>
-    <mergeCell ref="C3584:E3592"/>
-    <mergeCell ref="D3620:E3620"/>
-    <mergeCell ref="B3633:E3633"/>
-    <mergeCell ref="C3635:E3644"/>
-    <mergeCell ref="C3926:E3942"/>
-    <mergeCell ref="D3761:E3761"/>
-    <mergeCell ref="E3765:E3766"/>
-    <mergeCell ref="E3769:E3770"/>
-    <mergeCell ref="C3776:E3782"/>
-    <mergeCell ref="C3784:E3792"/>
-    <mergeCell ref="C3794:E3804"/>
-    <mergeCell ref="D3667:E3667"/>
-    <mergeCell ref="C3684:E3697"/>
-    <mergeCell ref="D3714:E3714"/>
-    <mergeCell ref="C3734:E3747"/>
-    <mergeCell ref="B3732:E3732"/>
-    <mergeCell ref="E3725:E3726"/>
-    <mergeCell ref="D3432:E3432"/>
-    <mergeCell ref="B3441:E3441"/>
-    <mergeCell ref="C3443:E3449"/>
-    <mergeCell ref="D3479:E3479"/>
-    <mergeCell ref="E3484:E3485"/>
-    <mergeCell ref="B3489:E3489"/>
-    <mergeCell ref="C3491:E3497"/>
-    <mergeCell ref="D3385:E3385"/>
-    <mergeCell ref="C3396:E3404"/>
-    <mergeCell ref="D1364:E1364"/>
-    <mergeCell ref="C1671:E1687"/>
-    <mergeCell ref="B1569:E1569"/>
-    <mergeCell ref="C1571:E1584"/>
-    <mergeCell ref="D1646:E1646"/>
-    <mergeCell ref="E1661:E1663"/>
-    <mergeCell ref="B1669:E1669"/>
-    <mergeCell ref="B1478:E1478"/>
-    <mergeCell ref="C1480:E1494"/>
-    <mergeCell ref="D1505:E1505"/>
-    <mergeCell ref="C1522:E1535"/>
-    <mergeCell ref="D1552:E1552"/>
-    <mergeCell ref="D1599:E1599"/>
-    <mergeCell ref="C1613:E1629"/>
-    <mergeCell ref="E1471:E1472"/>
-    <mergeCell ref="C1194:E1205"/>
-    <mergeCell ref="D1223:E1223"/>
-    <mergeCell ref="C1232:E1238"/>
-    <mergeCell ref="D1270:E1270"/>
-    <mergeCell ref="C1102:E1115"/>
-    <mergeCell ref="D1129:E1129"/>
-    <mergeCell ref="C1138:E1145"/>
-    <mergeCell ref="D1176:E1176"/>
-    <mergeCell ref="E1184:E1185"/>
-    <mergeCell ref="B1192:E1192"/>
-    <mergeCell ref="E1283:E1284"/>
-    <mergeCell ref="E1424:E1425"/>
-    <mergeCell ref="C1431:E1445"/>
-    <mergeCell ref="D1458:E1458"/>
-    <mergeCell ref="E1372:E1373"/>
-    <mergeCell ref="B1380:E1380"/>
-    <mergeCell ref="C1382:E1393"/>
-    <mergeCell ref="D1411:E1411"/>
-    <mergeCell ref="B1290:E1290"/>
-    <mergeCell ref="C1292:E1306"/>
-    <mergeCell ref="D1317:E1317"/>
-    <mergeCell ref="E1325:E1326"/>
-    <mergeCell ref="C1333:E1343"/>
-    <mergeCell ref="D1035:E1035"/>
-    <mergeCell ref="E1046:E1047"/>
-    <mergeCell ref="C1053:E1066"/>
-    <mergeCell ref="D1082:E1082"/>
-    <mergeCell ref="B1100:E1100"/>
-    <mergeCell ref="D941:E941"/>
-    <mergeCell ref="D988:E988"/>
-    <mergeCell ref="B1001:E1001"/>
-    <mergeCell ref="C1003:E1013"/>
-    <mergeCell ref="C954:E964"/>
-    <mergeCell ref="E1093:E1094"/>
-    <mergeCell ref="E670:E671"/>
-    <mergeCell ref="C677:E690"/>
-    <mergeCell ref="E717:E718"/>
-    <mergeCell ref="C820:E831"/>
-    <mergeCell ref="D894:E894"/>
-    <mergeCell ref="B916:E916"/>
-    <mergeCell ref="C918:E934"/>
-    <mergeCell ref="C768:E774"/>
-    <mergeCell ref="C776:E784"/>
-    <mergeCell ref="C786:E796"/>
-    <mergeCell ref="E757:E758"/>
-    <mergeCell ref="D800:E800"/>
-    <mergeCell ref="B818:E818"/>
-    <mergeCell ref="E810:E811"/>
-    <mergeCell ref="D847:E847"/>
-    <mergeCell ref="C861:E877"/>
-    <mergeCell ref="E909:E910"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="D283:E283"/>
-    <mergeCell ref="E292:E293"/>
-    <mergeCell ref="C299:E310"/>
-    <mergeCell ref="D330:E330"/>
-    <mergeCell ref="B346:E346"/>
-    <mergeCell ref="D189:E189"/>
-    <mergeCell ref="C200:E208"/>
-    <mergeCell ref="D236:E236"/>
-    <mergeCell ref="B247:E247"/>
-    <mergeCell ref="C249:E257"/>
-    <mergeCell ref="B65:E65"/>
-    <mergeCell ref="D142:E142"/>
-    <mergeCell ref="B164:E164"/>
-    <mergeCell ref="C166:E182"/>
-    <mergeCell ref="C67:E80"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="B25:E30"/>
-    <mergeCell ref="C109:E125"/>
-    <mergeCell ref="C31:E44"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="E157:E158"/>
-    <mergeCell ref="E339:E340"/>
+  <mergeCells count="339">
+    <mergeCell ref="C4997:E5003"/>
+    <mergeCell ref="D5030:E5030"/>
+    <mergeCell ref="E5035:E5036"/>
+    <mergeCell ref="B5040:E5040"/>
+    <mergeCell ref="B5041:E5041"/>
+    <mergeCell ref="C5043:E5049"/>
+    <mergeCell ref="C4712:E4720"/>
+    <mergeCell ref="D4748:E4748"/>
+    <mergeCell ref="B4764:E4764"/>
+    <mergeCell ref="D4936:E4936"/>
+    <mergeCell ref="B4950:E4950"/>
+    <mergeCell ref="C4952:E4958"/>
+    <mergeCell ref="D4983:E4983"/>
+    <mergeCell ref="B4995:E4995"/>
+    <mergeCell ref="C3257:E3265"/>
+    <mergeCell ref="D3291:E3291"/>
+    <mergeCell ref="C3306:E3317"/>
+    <mergeCell ref="D3338:E3338"/>
+    <mergeCell ref="B3354:E3354"/>
+    <mergeCell ref="C3356:E3367"/>
+    <mergeCell ref="C3117:E3133"/>
+    <mergeCell ref="D3150:E3150"/>
+    <mergeCell ref="B3172:E3172"/>
+    <mergeCell ref="C3174:E3190"/>
+    <mergeCell ref="D3197:E3197"/>
+    <mergeCell ref="C3208:E3216"/>
+    <mergeCell ref="D3244:E3244"/>
+    <mergeCell ref="B3255:E3255"/>
+    <mergeCell ref="E3165:E3166"/>
+    <mergeCell ref="E3347:E3348"/>
+    <mergeCell ref="C2985:E2999"/>
+    <mergeCell ref="B2983:E2983"/>
+    <mergeCell ref="D3009:E3009"/>
+    <mergeCell ref="E3018:E3019"/>
+    <mergeCell ref="C3027:E3040"/>
+    <mergeCell ref="D3056:E3056"/>
+    <mergeCell ref="B3073:E3073"/>
+    <mergeCell ref="C3075:E3088"/>
+    <mergeCell ref="D3103:E3103"/>
+    <mergeCell ref="B2884:E2884"/>
+    <mergeCell ref="C2886:E2896"/>
+    <mergeCell ref="D2915:E2915"/>
+    <mergeCell ref="C2935:E2949"/>
+    <mergeCell ref="D2962:E2962"/>
+    <mergeCell ref="E2975:E2977"/>
+    <mergeCell ref="E2787:E2789"/>
+    <mergeCell ref="B2795:E2795"/>
+    <mergeCell ref="C2797:E2811"/>
+    <mergeCell ref="D2821:E2821"/>
+    <mergeCell ref="E2829:E2830"/>
+    <mergeCell ref="C2837:E2847"/>
+    <mergeCell ref="D2868:E2868"/>
+    <mergeCell ref="E2876:E2877"/>
+    <mergeCell ref="E2928:E2929"/>
+    <mergeCell ref="D2633:E2633"/>
+    <mergeCell ref="C2642:E2649"/>
+    <mergeCell ref="D2680:E2680"/>
+    <mergeCell ref="E2688:E2689"/>
+    <mergeCell ref="B2696:E2696"/>
+    <mergeCell ref="C2698:E2709"/>
+    <mergeCell ref="D2727:E2727"/>
+    <mergeCell ref="C2736:E2742"/>
+    <mergeCell ref="D2774:E2774"/>
+    <mergeCell ref="D2539:E2539"/>
+    <mergeCell ref="C2557:E2570"/>
+    <mergeCell ref="D2586:E2586"/>
+    <mergeCell ref="C2607:E2620"/>
+    <mergeCell ref="E2597:E2599"/>
+    <mergeCell ref="B2605:E2605"/>
+    <mergeCell ref="D2398:E2398"/>
+    <mergeCell ref="E2413:E2415"/>
+    <mergeCell ref="B2421:E2421"/>
+    <mergeCell ref="C2423:E2439"/>
+    <mergeCell ref="D2445:E2445"/>
+    <mergeCell ref="C2458:E2468"/>
+    <mergeCell ref="D2492:E2492"/>
+    <mergeCell ref="B2505:E2505"/>
+    <mergeCell ref="C2507:E2517"/>
+    <mergeCell ref="E2550:E2551"/>
+    <mergeCell ref="C2280:E2288"/>
+    <mergeCell ref="C2290:E2300"/>
+    <mergeCell ref="D2304:E2304"/>
+    <mergeCell ref="E2314:E2315"/>
+    <mergeCell ref="B2322:E2322"/>
+    <mergeCell ref="C2324:E2337"/>
+    <mergeCell ref="D2351:E2351"/>
+    <mergeCell ref="C2365:E2381"/>
+    <mergeCell ref="D2210:E2210"/>
+    <mergeCell ref="E2221:E2223"/>
+    <mergeCell ref="C2231:E2244"/>
+    <mergeCell ref="B2229:E2229"/>
+    <mergeCell ref="D2257:E2257"/>
+    <mergeCell ref="E2261:E2262"/>
+    <mergeCell ref="E2265:E2266"/>
+    <mergeCell ref="C2272:E2278"/>
+    <mergeCell ref="D2069:E2069"/>
+    <mergeCell ref="C2084:E2094"/>
+    <mergeCell ref="D2116:E2116"/>
+    <mergeCell ref="C2131:E2141"/>
+    <mergeCell ref="B2129:E2129"/>
+    <mergeCell ref="D2163:E2163"/>
+    <mergeCell ref="C2181:E2194"/>
+    <mergeCell ref="D1975:E1975"/>
+    <mergeCell ref="D2022:E2022"/>
+    <mergeCell ref="E2174:E2175"/>
+    <mergeCell ref="E2027:E2028"/>
+    <mergeCell ref="B2032:E2032"/>
+    <mergeCell ref="B2033:E2033"/>
+    <mergeCell ref="C2035:E2041"/>
+    <mergeCell ref="C2043:E2056"/>
+    <mergeCell ref="C2057:E2057"/>
+    <mergeCell ref="D1787:E1787"/>
+    <mergeCell ref="C1803:E1814"/>
+    <mergeCell ref="D1834:E1834"/>
+    <mergeCell ref="E1843:E1845"/>
+    <mergeCell ref="C1853:E1864"/>
+    <mergeCell ref="E1796:E1797"/>
+    <mergeCell ref="E1980:E1981"/>
+    <mergeCell ref="C1985:E1991"/>
+    <mergeCell ref="B1851:E1851"/>
+    <mergeCell ref="C1894:E1904"/>
+    <mergeCell ref="D1928:E1928"/>
+    <mergeCell ref="B1937:E1937"/>
+    <mergeCell ref="C1939:E1945"/>
+    <mergeCell ref="C348:E359"/>
+    <mergeCell ref="D377:E377"/>
+    <mergeCell ref="C388:E396"/>
+    <mergeCell ref="C553:E553"/>
+    <mergeCell ref="D565:E565"/>
+    <mergeCell ref="C578:E588"/>
+    <mergeCell ref="D612:E612"/>
+    <mergeCell ref="D518:E518"/>
+    <mergeCell ref="E523:E524"/>
     <mergeCell ref="D1693:E1693"/>
     <mergeCell ref="C1706:E1714"/>
     <mergeCell ref="D1740:E1740"/>
@@ -30357,125 +30987,178 @@
     <mergeCell ref="C627:E636"/>
     <mergeCell ref="B625:E625"/>
     <mergeCell ref="D659:E659"/>
-    <mergeCell ref="C348:E359"/>
-    <mergeCell ref="D377:E377"/>
-    <mergeCell ref="C388:E396"/>
-    <mergeCell ref="C553:E553"/>
-    <mergeCell ref="D565:E565"/>
-    <mergeCell ref="C578:E588"/>
-    <mergeCell ref="D612:E612"/>
-    <mergeCell ref="D518:E518"/>
-    <mergeCell ref="E523:E524"/>
-    <mergeCell ref="D1787:E1787"/>
-    <mergeCell ref="C1803:E1814"/>
-    <mergeCell ref="D1834:E1834"/>
-    <mergeCell ref="E1843:E1845"/>
-    <mergeCell ref="C1853:E1864"/>
-    <mergeCell ref="E1796:E1797"/>
-    <mergeCell ref="E1980:E1981"/>
-    <mergeCell ref="C1985:E1991"/>
-    <mergeCell ref="B1851:E1851"/>
-    <mergeCell ref="D2069:E2069"/>
-    <mergeCell ref="C2084:E2094"/>
-    <mergeCell ref="D2116:E2116"/>
-    <mergeCell ref="C2131:E2141"/>
-    <mergeCell ref="B2129:E2129"/>
-    <mergeCell ref="D2163:E2163"/>
-    <mergeCell ref="C2181:E2194"/>
-    <mergeCell ref="D1975:E1975"/>
-    <mergeCell ref="D2022:E2022"/>
-    <mergeCell ref="E2174:E2175"/>
-    <mergeCell ref="E2027:E2028"/>
-    <mergeCell ref="B2032:E2032"/>
-    <mergeCell ref="B2033:E2033"/>
-    <mergeCell ref="C2035:E2041"/>
-    <mergeCell ref="C2043:E2056"/>
-    <mergeCell ref="C2057:E2057"/>
-    <mergeCell ref="C1894:E1904"/>
-    <mergeCell ref="D1928:E1928"/>
-    <mergeCell ref="B1937:E1937"/>
-    <mergeCell ref="C1939:E1945"/>
-    <mergeCell ref="C2280:E2288"/>
-    <mergeCell ref="C2290:E2300"/>
-    <mergeCell ref="D2304:E2304"/>
-    <mergeCell ref="E2314:E2315"/>
-    <mergeCell ref="B2322:E2322"/>
-    <mergeCell ref="C2324:E2337"/>
-    <mergeCell ref="D2351:E2351"/>
-    <mergeCell ref="C2365:E2381"/>
-    <mergeCell ref="D2210:E2210"/>
-    <mergeCell ref="E2221:E2223"/>
-    <mergeCell ref="C2231:E2244"/>
-    <mergeCell ref="B2229:E2229"/>
-    <mergeCell ref="D2257:E2257"/>
-    <mergeCell ref="E2261:E2262"/>
-    <mergeCell ref="E2265:E2266"/>
-    <mergeCell ref="C2272:E2278"/>
-    <mergeCell ref="D2539:E2539"/>
-    <mergeCell ref="C2557:E2570"/>
-    <mergeCell ref="D2586:E2586"/>
-    <mergeCell ref="C2607:E2620"/>
-    <mergeCell ref="E2597:E2599"/>
-    <mergeCell ref="B2605:E2605"/>
-    <mergeCell ref="D2398:E2398"/>
-    <mergeCell ref="E2413:E2415"/>
-    <mergeCell ref="B2421:E2421"/>
-    <mergeCell ref="C2423:E2439"/>
-    <mergeCell ref="D2445:E2445"/>
-    <mergeCell ref="C2458:E2468"/>
-    <mergeCell ref="D2492:E2492"/>
-    <mergeCell ref="B2505:E2505"/>
-    <mergeCell ref="C2507:E2517"/>
-    <mergeCell ref="E2550:E2551"/>
-    <mergeCell ref="D2633:E2633"/>
-    <mergeCell ref="C2642:E2649"/>
-    <mergeCell ref="D2680:E2680"/>
-    <mergeCell ref="E2688:E2689"/>
-    <mergeCell ref="B2696:E2696"/>
-    <mergeCell ref="C2698:E2709"/>
-    <mergeCell ref="D2727:E2727"/>
-    <mergeCell ref="C2736:E2742"/>
-    <mergeCell ref="D2774:E2774"/>
-    <mergeCell ref="B2884:E2884"/>
-    <mergeCell ref="C2886:E2896"/>
-    <mergeCell ref="D2915:E2915"/>
-    <mergeCell ref="C2935:E2949"/>
-    <mergeCell ref="D2962:E2962"/>
-    <mergeCell ref="E2975:E2977"/>
-    <mergeCell ref="E2787:E2789"/>
-    <mergeCell ref="B2795:E2795"/>
-    <mergeCell ref="C2797:E2811"/>
-    <mergeCell ref="D2821:E2821"/>
-    <mergeCell ref="E2829:E2830"/>
-    <mergeCell ref="C2837:E2847"/>
-    <mergeCell ref="D2868:E2868"/>
-    <mergeCell ref="E2876:E2877"/>
-    <mergeCell ref="E2928:E2929"/>
-    <mergeCell ref="C2985:E2999"/>
-    <mergeCell ref="B2983:E2983"/>
-    <mergeCell ref="D3009:E3009"/>
-    <mergeCell ref="E3018:E3019"/>
-    <mergeCell ref="C3027:E3040"/>
-    <mergeCell ref="D3056:E3056"/>
-    <mergeCell ref="B3073:E3073"/>
-    <mergeCell ref="C3075:E3088"/>
-    <mergeCell ref="D3103:E3103"/>
-    <mergeCell ref="C3257:E3265"/>
-    <mergeCell ref="D3291:E3291"/>
-    <mergeCell ref="C3306:E3317"/>
-    <mergeCell ref="D3338:E3338"/>
-    <mergeCell ref="B3354:E3354"/>
-    <mergeCell ref="C3356:E3367"/>
-    <mergeCell ref="C3117:E3133"/>
-    <mergeCell ref="D3150:E3150"/>
-    <mergeCell ref="B3172:E3172"/>
-    <mergeCell ref="C3174:E3190"/>
-    <mergeCell ref="D3197:E3197"/>
-    <mergeCell ref="C3208:E3216"/>
-    <mergeCell ref="D3244:E3244"/>
-    <mergeCell ref="B3255:E3255"/>
-    <mergeCell ref="E3165:E3166"/>
-    <mergeCell ref="E3347:E3348"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="D283:E283"/>
+    <mergeCell ref="E292:E293"/>
+    <mergeCell ref="C299:E310"/>
+    <mergeCell ref="D330:E330"/>
+    <mergeCell ref="B346:E346"/>
+    <mergeCell ref="D189:E189"/>
+    <mergeCell ref="C200:E208"/>
+    <mergeCell ref="D236:E236"/>
+    <mergeCell ref="B247:E247"/>
+    <mergeCell ref="C249:E257"/>
+    <mergeCell ref="B65:E65"/>
+    <mergeCell ref="D142:E142"/>
+    <mergeCell ref="B164:E164"/>
+    <mergeCell ref="C166:E182"/>
+    <mergeCell ref="C67:E80"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="B25:E30"/>
+    <mergeCell ref="C109:E125"/>
+    <mergeCell ref="C31:E44"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="E157:E158"/>
+    <mergeCell ref="E339:E340"/>
+    <mergeCell ref="E670:E671"/>
+    <mergeCell ref="C677:E690"/>
+    <mergeCell ref="E717:E718"/>
+    <mergeCell ref="C820:E831"/>
+    <mergeCell ref="D894:E894"/>
+    <mergeCell ref="B916:E916"/>
+    <mergeCell ref="C918:E934"/>
+    <mergeCell ref="C768:E774"/>
+    <mergeCell ref="C776:E784"/>
+    <mergeCell ref="C786:E796"/>
+    <mergeCell ref="E757:E758"/>
+    <mergeCell ref="D800:E800"/>
+    <mergeCell ref="B818:E818"/>
+    <mergeCell ref="E810:E811"/>
+    <mergeCell ref="D847:E847"/>
+    <mergeCell ref="C861:E877"/>
+    <mergeCell ref="E909:E910"/>
+    <mergeCell ref="D1035:E1035"/>
+    <mergeCell ref="E1046:E1047"/>
+    <mergeCell ref="C1053:E1066"/>
+    <mergeCell ref="D1082:E1082"/>
+    <mergeCell ref="B1100:E1100"/>
+    <mergeCell ref="D941:E941"/>
+    <mergeCell ref="D988:E988"/>
+    <mergeCell ref="B1001:E1001"/>
+    <mergeCell ref="C1003:E1013"/>
+    <mergeCell ref="C954:E964"/>
+    <mergeCell ref="E1093:E1094"/>
+    <mergeCell ref="E1283:E1284"/>
+    <mergeCell ref="E1424:E1425"/>
+    <mergeCell ref="C1431:E1445"/>
+    <mergeCell ref="D1458:E1458"/>
+    <mergeCell ref="E1372:E1373"/>
+    <mergeCell ref="B1380:E1380"/>
+    <mergeCell ref="C1382:E1393"/>
+    <mergeCell ref="D1411:E1411"/>
+    <mergeCell ref="B1290:E1290"/>
+    <mergeCell ref="C1292:E1306"/>
+    <mergeCell ref="D1317:E1317"/>
+    <mergeCell ref="E1325:E1326"/>
+    <mergeCell ref="C1333:E1343"/>
+    <mergeCell ref="C1194:E1205"/>
+    <mergeCell ref="D1223:E1223"/>
+    <mergeCell ref="C1232:E1238"/>
+    <mergeCell ref="D1270:E1270"/>
+    <mergeCell ref="C1102:E1115"/>
+    <mergeCell ref="D1129:E1129"/>
+    <mergeCell ref="C1138:E1145"/>
+    <mergeCell ref="D1176:E1176"/>
+    <mergeCell ref="E1184:E1185"/>
+    <mergeCell ref="B1192:E1192"/>
+    <mergeCell ref="D1364:E1364"/>
+    <mergeCell ref="C1671:E1687"/>
+    <mergeCell ref="B1569:E1569"/>
+    <mergeCell ref="C1571:E1584"/>
+    <mergeCell ref="D1646:E1646"/>
+    <mergeCell ref="E1661:E1663"/>
+    <mergeCell ref="B1669:E1669"/>
+    <mergeCell ref="B1478:E1478"/>
+    <mergeCell ref="C1480:E1494"/>
+    <mergeCell ref="D1505:E1505"/>
+    <mergeCell ref="C1522:E1535"/>
+    <mergeCell ref="D1552:E1552"/>
+    <mergeCell ref="D1599:E1599"/>
+    <mergeCell ref="C1613:E1629"/>
+    <mergeCell ref="E1471:E1472"/>
+    <mergeCell ref="D3432:E3432"/>
+    <mergeCell ref="B3441:E3441"/>
+    <mergeCell ref="C3443:E3449"/>
+    <mergeCell ref="D3479:E3479"/>
+    <mergeCell ref="E3484:E3485"/>
+    <mergeCell ref="B3489:E3489"/>
+    <mergeCell ref="C3491:E3497"/>
+    <mergeCell ref="D3385:E3385"/>
+    <mergeCell ref="C3396:E3404"/>
+    <mergeCell ref="D3573:E3573"/>
+    <mergeCell ref="D3526:E3526"/>
+    <mergeCell ref="E3531:E3532"/>
+    <mergeCell ref="C3536:E3542"/>
+    <mergeCell ref="C3584:E3592"/>
+    <mergeCell ref="D3620:E3620"/>
+    <mergeCell ref="B3633:E3633"/>
+    <mergeCell ref="C3635:E3644"/>
+    <mergeCell ref="C3926:E3942"/>
+    <mergeCell ref="D3761:E3761"/>
+    <mergeCell ref="E3765:E3766"/>
+    <mergeCell ref="E3769:E3770"/>
+    <mergeCell ref="C3776:E3782"/>
+    <mergeCell ref="C3784:E3792"/>
+    <mergeCell ref="C3794:E3804"/>
+    <mergeCell ref="D3667:E3667"/>
+    <mergeCell ref="C3684:E3697"/>
+    <mergeCell ref="D3714:E3714"/>
+    <mergeCell ref="C3734:E3747"/>
+    <mergeCell ref="B3732:E3732"/>
+    <mergeCell ref="E3725:E3726"/>
+    <mergeCell ref="D3949:E3949"/>
+    <mergeCell ref="C3962:E3972"/>
+    <mergeCell ref="D3996:E3996"/>
+    <mergeCell ref="C4011:E4021"/>
+    <mergeCell ref="B4009:E4009"/>
+    <mergeCell ref="D4043:E4043"/>
+    <mergeCell ref="C4060:E4073"/>
+    <mergeCell ref="D3808:E3808"/>
+    <mergeCell ref="E3818:E3819"/>
+    <mergeCell ref="B3826:E3826"/>
+    <mergeCell ref="C3828:E3839"/>
+    <mergeCell ref="D3855:E3855"/>
+    <mergeCell ref="C3869:E3885"/>
+    <mergeCell ref="D3902:E3902"/>
+    <mergeCell ref="E3917:E3918"/>
+    <mergeCell ref="B3924:E3924"/>
+    <mergeCell ref="B4108:E4108"/>
+    <mergeCell ref="D4325:E4325"/>
+    <mergeCell ref="D4090:E4090"/>
+    <mergeCell ref="C4110:E4123"/>
+    <mergeCell ref="E4101:E4102"/>
+    <mergeCell ref="D4137:E4137"/>
+    <mergeCell ref="C4146:E4153"/>
+    <mergeCell ref="D4184:E4184"/>
+    <mergeCell ref="E4192:E4193"/>
+    <mergeCell ref="B4200:E4200"/>
+    <mergeCell ref="C4202:E4213"/>
+    <mergeCell ref="E4333:E4334"/>
+    <mergeCell ref="C4341:E4352"/>
+    <mergeCell ref="D4372:E4372"/>
+    <mergeCell ref="E4380:E4381"/>
+    <mergeCell ref="C4390:E4401"/>
+    <mergeCell ref="B4388:E4388"/>
+    <mergeCell ref="D4231:E4231"/>
+    <mergeCell ref="C4240:E4246"/>
+    <mergeCell ref="D4278:E4278"/>
+    <mergeCell ref="E4291:E4292"/>
+    <mergeCell ref="B4298:E4298"/>
+    <mergeCell ref="C4300:E4314"/>
+    <mergeCell ref="C4902:E4912"/>
+    <mergeCell ref="C4530:E4543"/>
+    <mergeCell ref="D4560:E4560"/>
+    <mergeCell ref="B4582:E4582"/>
+    <mergeCell ref="C4584:E4597"/>
+    <mergeCell ref="D4607:E4607"/>
+    <mergeCell ref="C4621:E4637"/>
+    <mergeCell ref="D4419:E4419"/>
+    <mergeCell ref="C4438:E4452"/>
+    <mergeCell ref="D4466:E4466"/>
+    <mergeCell ref="C4488:E4502"/>
+    <mergeCell ref="E4479:E4480"/>
+    <mergeCell ref="B4486:E4486"/>
+    <mergeCell ref="D4513:E4513"/>
     <mergeCell ref="C4766:E4774"/>
     <mergeCell ref="D4795:E4795"/>
     <mergeCell ref="C4813:E4824"/>
@@ -30486,9 +31169,6 @@
     <mergeCell ref="B4678:E4678"/>
     <mergeCell ref="C4680:E4696"/>
     <mergeCell ref="D4701:E4701"/>
-    <mergeCell ref="C4712:E4720"/>
-    <mergeCell ref="D4748:E4748"/>
-    <mergeCell ref="B4764:E4764"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Phosphor decay added to L. Spiro NTSC.  PAL CRT added AVX.
</commit_message>
<xml_diff>
--- a/Research/Instructions/Instructions New NES.xlsx
+++ b/Research/Instructions/Instructions New NES.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Projects\BeesNES\Research\Instructions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC5AEB2-808E-47BC-9807-FC501D933800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE53AA3-AD5F-488F-BFC8-44FEE8F29B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{7ED93F2B-FF78-48E4-8428-9E2E36877943}"/>
+    <workbookView xWindow="3105" yWindow="0" windowWidth="28800" windowHeight="20985" xr2:uid="{7ED93F2B-FF78-48E4-8428-9E2E36877943}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$5075</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$5074</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="108">
+  <futureMetadata name="XLRICHVALUE" count="109">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -800,8 +800,15 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="108"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="108">
+  <valueMetadata count="109">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -1126,12 +1133,15 @@
     <bk>
       <rc t="1" v="107"/>
     </bk>
+    <bk>
+      <rc t="1" v="108"/>
+    </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2681" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2685" uniqueCount="276">
   <si>
     <t>BRK (00)</t>
   </si>
@@ -6157,6 +6167,306 @@
   </si>
   <si>
     <t>ARR (6B)</t>
+  </si>
+  <si>
+    <r>
+      <t>Tmp = (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;&lt; 7).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Set </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> if highest bit of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is set.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Inc. PC. * Perform </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &amp; Operand.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &gt;&gt; 1) | Tmp.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Set </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> as (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ^ ((</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &gt;&gt; 5) &amp; 1)) != 0.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Set </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Z</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>N</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> based off </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -6665,7 +6975,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="108">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="109">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -7098,6 +7408,10 @@
     <v>107</v>
     <v>5</v>
   </rv>
+  <rv s="0">
+    <v>108</v>
+    <v>5</v>
+  </rv>
 </rvData>
 </file>
 
@@ -7220,6 +7534,7 @@
   <rel r:id="rId106"/>
   <rel r:id="rId107"/>
   <rel r:id="rId108"/>
+  <rel r:id="rId109"/>
 </richValueRels>
 </file>
 
@@ -7540,10 +7855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236A51FB-68FA-4644-A8C6-D47AA32EBCC5}">
-  <dimension ref="B1:F5049"/>
+  <dimension ref="B1:F5052"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5007" zoomScale="115" zoomScaleNormal="55" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="C5030" sqref="C5030"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5019" zoomScale="115" zoomScaleNormal="55" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="J5043" sqref="J5043"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -30681,7 +30996,7 @@
       <c r="D5003" s="43"/>
       <c r="E5003" s="43"/>
     </row>
-    <row r="5029" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5029" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5029" s="1" t="s">
         <v>269</v>
       </c>
@@ -30692,14 +31007,14 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5030" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5030" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5030" s="21"/>
       <c r="D5030" s="45" t="s">
         <v>56</v>
       </c>
       <c r="E5030" s="46"/>
     </row>
-    <row r="5031" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5031" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5031" s="7" t="s">
         <v>4</v>
       </c>
@@ -30710,7 +31025,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5032" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5032" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5032" s="20" t="s">
         <v>12</v>
       </c>
@@ -30721,7 +31036,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5033" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5033" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5033" s="9">
         <v>1.1000000000000001</v>
       </c>
@@ -30730,7 +31045,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5034" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5034" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5034" s="40">
         <v>1.2</v>
       </c>
@@ -30741,75 +31056,82 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5035" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5035" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5035" s="9">
         <v>2.1</v>
       </c>
       <c r="D5035" s="10"/>
-      <c r="E5035" s="48" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="5036" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5035" s="22" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="5036" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5036" s="9"/>
       <c r="D5036" s="10"/>
-      <c r="E5036" s="48"/>
-    </row>
-    <row r="5037" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5037" s="9">
+      <c r="E5036" s="22" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="5037" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5037" s="9"/>
+      <c r="D5037" s="10"/>
+      <c r="E5037" s="22" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="5038" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5038" s="9"/>
+      <c r="D5038" s="10"/>
+      <c r="E5038" s="22" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="5039" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5039" s="9"/>
+      <c r="D5039" s="10"/>
+      <c r="E5039" s="22" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="5040" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5040" s="9"/>
+      <c r="D5040" s="10"/>
+      <c r="E5040" s="22" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="5041" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5041" s="9">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D5037" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5037" s="11" t="s">
+      <c r="D5041" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5041" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5038" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5038" s="15" t="s">
+    <row r="5042" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5042" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D5038" s="16"/>
-      <c r="E5038" s="17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5040" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5040" s="47" t="s">
+      <c r="D5042" s="16"/>
+      <c r="E5042" s="17" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="5044" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5044" s="47" t="s">
         <v>43</v>
       </c>
-      <c r="C5040" s="47"/>
-      <c r="D5040" s="47"/>
-      <c r="E5040" s="47"/>
-    </row>
-    <row r="5041" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5041" s="50" t="s">
-        <v>171</v>
-      </c>
-      <c r="C5041" s="50"/>
-      <c r="D5041" s="50"/>
-      <c r="E5041" s="50"/>
-    </row>
-    <row r="5043" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5043" s="43" t="e" vm="12">
+      <c r="C5044" s="47"/>
+      <c r="D5044" s="47"/>
+      <c r="E5044" s="47"/>
+    </row>
+    <row r="5046" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5046" s="43" t="e" vm="109">
         <v>#VALUE!</v>
       </c>
-      <c r="D5043" s="43"/>
-      <c r="E5043" s="43"/>
-    </row>
-    <row r="5044" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5044" s="43"/>
-      <c r="D5044" s="43"/>
-      <c r="E5044" s="43"/>
-    </row>
-    <row r="5045" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5045" s="43"/>
-      <c r="D5045" s="43"/>
-      <c r="E5045" s="43"/>
-    </row>
-    <row r="5046" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5046" s="43"/>
       <c r="D5046" s="43"/>
       <c r="E5046" s="43"/>
     </row>
@@ -30828,14 +31150,27 @@
       <c r="D5049" s="43"/>
       <c r="E5049" s="43"/>
     </row>
+    <row r="5050" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5050" s="43"/>
+      <c r="D5050" s="43"/>
+      <c r="E5050" s="43"/>
+    </row>
+    <row r="5051" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5051" s="43"/>
+      <c r="D5051" s="43"/>
+      <c r="E5051" s="43"/>
+    </row>
+    <row r="5052" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5052" s="43"/>
+      <c r="D5052" s="43"/>
+      <c r="E5052" s="43"/>
+    </row>
   </sheetData>
-  <mergeCells count="339">
+  <mergeCells count="337">
     <mergeCell ref="C4997:E5003"/>
     <mergeCell ref="D5030:E5030"/>
-    <mergeCell ref="E5035:E5036"/>
-    <mergeCell ref="B5040:E5040"/>
-    <mergeCell ref="B5041:E5041"/>
-    <mergeCell ref="C5043:E5049"/>
+    <mergeCell ref="B5044:E5044"/>
+    <mergeCell ref="C5046:E5052"/>
     <mergeCell ref="C4712:E4720"/>
     <mergeCell ref="D4748:E4748"/>
     <mergeCell ref="B4764:E4764"/>

</xml_diff>

<commit_message>
Added instruction descriptions, WAV Editor fixes.
</commit_message>
<xml_diff>
--- a/Research/Instructions/Instructions New NES.xlsx
+++ b/Research/Instructions/Instructions New NES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Projects\BeesNES\Research\Instructions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{88B92563-66AE-46A4-9B0B-C7418FD45D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{B91E0C9E-CF02-43EF-ACDF-FA91208261D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16110" yWindow="0" windowWidth="22395" windowHeight="20985" xr2:uid="{7ED93F2B-FF78-48E4-8428-9E2E36877943}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$5169</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$5216</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -44,7 +44,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="110">
+  <futureMetadata name="XLRICHVALUE" count="112">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -815,8 +815,22 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="110"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="111"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="110">
+  <valueMetadata count="112">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -1147,12 +1161,18 @@
     <bk>
       <rc t="1" v="109"/>
     </bk>
+    <bk>
+      <rc t="1" v="110"/>
+    </bk>
+    <bk>
+      <rc t="1" v="111"/>
+    </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2712" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2772" uniqueCount="289">
   <si>
     <t>BRK (00)</t>
   </si>
@@ -7177,6 +7197,12 @@
   </si>
   <si>
     <t>* Read operation does not cross into a new page if (Pointer+1) causes overflow, hence the high byte of Pointer is retained while “+ 1” is applied only to the low byte.</t>
+  </si>
+  <si>
+    <t>ADC (6D)</t>
+  </si>
+  <si>
+    <t>ROR (6E)</t>
   </si>
 </sst>
 </file>
@@ -7682,7 +7708,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="110">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="112">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -8123,6 +8149,14 @@
     <v>109</v>
     <v>5</v>
   </rv>
+  <rv s="0">
+    <v>110</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>111</v>
+    <v>5</v>
+  </rv>
 </rvData>
 </file>
 
@@ -8247,6 +8281,8 @@
   <rel r:id="rId108"/>
   <rel r:id="rId109"/>
   <rel r:id="rId110"/>
+  <rel r:id="rId111"/>
+  <rel r:id="rId112"/>
 </richValueRels>
 </file>
 
@@ -8567,10 +8603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236A51FB-68FA-4644-A8C6-D47AA32EBCC5}">
-  <dimension ref="B1:F5109"/>
+  <dimension ref="B1:F5204"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5074" zoomScale="115" zoomScaleNormal="55" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="C5108" sqref="C5108:E5109"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5177" zoomScale="115" zoomScaleNormal="55" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="E5182" sqref="E5182:E5185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -32114,13 +32150,508 @@
       <c r="D5109" s="48"/>
       <c r="E5109" s="48"/>
     </row>
+    <row r="5123" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5123" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="D5123" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5123" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5124" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5124" s="21"/>
+      <c r="D5124" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5124" s="43"/>
+    </row>
+    <row r="5125" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5125" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5125" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5125" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5126" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5126" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5126" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5126" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5127" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5127" s="9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D5127" s="10"/>
+      <c r="E5127" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5128" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5128" s="9">
+        <v>1.2</v>
+      </c>
+      <c r="D5128" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5128" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5129" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5129" s="9">
+        <v>2.1</v>
+      </c>
+      <c r="D5129" s="10"/>
+      <c r="E5129" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5130" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5130" s="9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D5130" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5130" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5131" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5131" s="9">
+        <v>3.1</v>
+      </c>
+      <c r="D5131" s="10"/>
+      <c r="E5131" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5132" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5132" s="39">
+        <v>3.2</v>
+      </c>
+      <c r="D5132" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5132" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5133" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5133" s="9">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D5133" s="10"/>
+      <c r="E5133" s="22" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="5134" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5134" s="9"/>
+      <c r="D5134" s="10"/>
+      <c r="E5134" s="11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5135" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5135" s="9"/>
+      <c r="D5135" s="10"/>
+      <c r="E5135" s="22" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="5136" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5136" s="9"/>
+      <c r="D5136" s="10"/>
+      <c r="E5136" s="22" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5137" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5137" s="9"/>
+      <c r="D5137" s="10"/>
+      <c r="E5137" s="22" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5138" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5138" s="9"/>
+      <c r="D5138" s="10"/>
+      <c r="E5138" s="22" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="5139" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5139" s="9">
+        <v>4.2</v>
+      </c>
+      <c r="D5139" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5139" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5140" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5140" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5140" s="16"/>
+      <c r="E5140" s="17" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5141" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5141" s="19"/>
+      <c r="D5141" s="23"/>
+      <c r="E5141" s="14"/>
+    </row>
+    <row r="5142" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5142" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5142" s="44"/>
+      <c r="D5142" s="44"/>
+      <c r="E5142" s="44"/>
+    </row>
+    <row r="5144" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5144" s="45" t="e" vm="111">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D5144" s="45"/>
+      <c r="E5144" s="45"/>
+    </row>
+    <row r="5145" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5145" s="45"/>
+      <c r="D5145" s="45"/>
+      <c r="E5145" s="45"/>
+    </row>
+    <row r="5146" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5146" s="45"/>
+      <c r="D5146" s="45"/>
+      <c r="E5146" s="45"/>
+    </row>
+    <row r="5147" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5147" s="45"/>
+      <c r="D5147" s="45"/>
+      <c r="E5147" s="45"/>
+    </row>
+    <row r="5148" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5148" s="45"/>
+      <c r="D5148" s="45"/>
+      <c r="E5148" s="45"/>
+    </row>
+    <row r="5149" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5149" s="45"/>
+      <c r="D5149" s="45"/>
+      <c r="E5149" s="45"/>
+    </row>
+    <row r="5150" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5150" s="45"/>
+      <c r="D5150" s="45"/>
+      <c r="E5150" s="45"/>
+    </row>
+    <row r="5151" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5151" s="45"/>
+      <c r="D5151" s="45"/>
+      <c r="E5151" s="45"/>
+    </row>
+    <row r="5152" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5152" s="45"/>
+      <c r="D5152" s="45"/>
+      <c r="E5152" s="45"/>
+    </row>
+    <row r="5153" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5153" s="45"/>
+      <c r="D5153" s="45"/>
+      <c r="E5153" s="45"/>
+    </row>
+    <row r="5154" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5154" s="45"/>
+      <c r="D5154" s="45"/>
+      <c r="E5154" s="45"/>
+    </row>
+    <row r="5170" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5170" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D5170" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5170" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5171" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5171" s="21"/>
+      <c r="D5171" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5171" s="43"/>
+    </row>
+    <row r="5172" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5172" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5172" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5172" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5173" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5173" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5173" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5173" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5174" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5174" s="9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D5174" s="10"/>
+      <c r="E5174" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5175" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5175" s="9">
+        <v>1.2</v>
+      </c>
+      <c r="D5175" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5175" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5176" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5176" s="9">
+        <v>2.1</v>
+      </c>
+      <c r="D5176" s="10"/>
+      <c r="E5176" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5177" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5177" s="9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D5177" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5177" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5178" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5178" s="9">
+        <v>3.1</v>
+      </c>
+      <c r="D5178" s="10"/>
+      <c r="E5178" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5179" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5179" s="9">
+        <v>3.2</v>
+      </c>
+      <c r="D5179" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5179" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5180" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5180" s="9">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D5180" s="10"/>
+      <c r="E5180" s="11"/>
+    </row>
+    <row r="5181" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5181" s="9">
+        <v>4.2</v>
+      </c>
+      <c r="D5181" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5181" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5182" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5182" s="9">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D5182" s="10"/>
+      <c r="E5182" s="22" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5183" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5183" s="9"/>
+      <c r="D5183" s="10"/>
+      <c r="E5183" s="22" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="5184" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5184" s="9"/>
+      <c r="D5184" s="10"/>
+      <c r="E5184" s="11" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5185" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5185" s="9"/>
+      <c r="D5185" s="10"/>
+      <c r="E5185" s="11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5186" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5186" s="39">
+        <v>5.2</v>
+      </c>
+      <c r="D5186" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5186" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5187" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5187" s="9">
+        <v>6.1</v>
+      </c>
+      <c r="D5187" s="10"/>
+      <c r="E5187" s="22"/>
+    </row>
+    <row r="5188" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5188" s="9">
+        <v>6.2</v>
+      </c>
+      <c r="D5188" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5188" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5189" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5189" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5189" s="16"/>
+      <c r="E5189" s="17"/>
+    </row>
+    <row r="5191" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5191" s="45" t="e" vm="112">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D5191" s="45"/>
+      <c r="E5191" s="45"/>
+    </row>
+    <row r="5192" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5192" s="45"/>
+      <c r="D5192" s="45"/>
+      <c r="E5192" s="45"/>
+    </row>
+    <row r="5193" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5193" s="45"/>
+      <c r="D5193" s="45"/>
+      <c r="E5193" s="45"/>
+    </row>
+    <row r="5194" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5194" s="45"/>
+      <c r="D5194" s="45"/>
+      <c r="E5194" s="45"/>
+    </row>
+    <row r="5195" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5195" s="45"/>
+      <c r="D5195" s="45"/>
+      <c r="E5195" s="45"/>
+    </row>
+    <row r="5196" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5196" s="45"/>
+      <c r="D5196" s="45"/>
+      <c r="E5196" s="45"/>
+    </row>
+    <row r="5197" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5197" s="45"/>
+      <c r="D5197" s="45"/>
+      <c r="E5197" s="45"/>
+    </row>
+    <row r="5198" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5198" s="45"/>
+      <c r="D5198" s="45"/>
+      <c r="E5198" s="45"/>
+    </row>
+    <row r="5199" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5199" s="45"/>
+      <c r="D5199" s="45"/>
+      <c r="E5199" s="45"/>
+    </row>
+    <row r="5200" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5200" s="45"/>
+      <c r="D5200" s="45"/>
+      <c r="E5200" s="45"/>
+    </row>
+    <row r="5201" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5201" s="45"/>
+      <c r="D5201" s="45"/>
+      <c r="E5201" s="45"/>
+    </row>
+    <row r="5202" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5202" s="45"/>
+      <c r="D5202" s="45"/>
+      <c r="E5202" s="45"/>
+    </row>
+    <row r="5203" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5203" s="45"/>
+      <c r="D5203" s="45"/>
+      <c r="E5203" s="45"/>
+    </row>
+    <row r="5204" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5204" s="45"/>
+      <c r="D5204" s="45"/>
+      <c r="E5204" s="45"/>
+    </row>
   </sheetData>
-  <mergeCells count="343">
+  <mergeCells count="348">
+    <mergeCell ref="B5142:E5142"/>
+    <mergeCell ref="C5144:E5154"/>
+    <mergeCell ref="D5171:E5171"/>
+    <mergeCell ref="C5191:E5204"/>
     <mergeCell ref="D5077:E5077"/>
     <mergeCell ref="E5086:E5087"/>
     <mergeCell ref="C5095:E5106"/>
     <mergeCell ref="D5088:D5090"/>
     <mergeCell ref="C5108:E5109"/>
+    <mergeCell ref="D5124:E5124"/>
     <mergeCell ref="C4997:E5003"/>
     <mergeCell ref="D5030:E5030"/>
     <mergeCell ref="B5044:E5044"/>

</xml_diff>

<commit_message>
Added documented instruction, WAV Editor functionality.
</commit_message>
<xml_diff>
--- a/Research/Instructions/Instructions New NES.xlsx
+++ b/Research/Instructions/Instructions New NES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Projects\BeesNES\Research\Instructions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{B91E0C9E-CF02-43EF-ACDF-FA91208261D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{B4983C94-65FA-4BF4-A88E-0B16A550F595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16110" yWindow="0" windowWidth="22395" windowHeight="20985" xr2:uid="{7ED93F2B-FF78-48E4-8428-9E2E36877943}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$5216</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$5260</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -44,7 +44,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="112">
+  <futureMetadata name="XLRICHVALUE" count="113">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -829,8 +829,15 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="112"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="112">
+  <valueMetadata count="113">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -1167,12 +1174,15 @@
     <bk>
       <rc t="1" v="111"/>
     </bk>
+    <bk>
+      <rc t="1" v="112"/>
+    </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2772" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2802" uniqueCount="290">
   <si>
     <t>BRK (00)</t>
   </si>
@@ -7203,6 +7213,9 @@
   </si>
   <si>
     <t>ROR (6E)</t>
+  </si>
+  <si>
+    <t>RRA (6F)</t>
   </si>
 </sst>
 </file>
@@ -7708,7 +7721,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="112">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="113">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -8157,6 +8170,10 @@
     <v>111</v>
     <v>5</v>
   </rv>
+  <rv s="0">
+    <v>112</v>
+    <v>5</v>
+  </rv>
 </rvData>
 </file>
 
@@ -8283,6 +8300,7 @@
   <rel r:id="rId110"/>
   <rel r:id="rId111"/>
   <rel r:id="rId112"/>
+  <rel r:id="rId113"/>
 </richValueRels>
 </file>
 
@@ -8603,10 +8621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{236A51FB-68FA-4644-A8C6-D47AA32EBCC5}">
-  <dimension ref="B1:F5204"/>
+  <dimension ref="B1:F5251"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5177" zoomScale="115" zoomScaleNormal="55" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="E5182" sqref="E5182:E5185"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5214" zoomScale="115" zoomScaleNormal="55" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="C5238" sqref="C5238:E5251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -32640,12 +32658,270 @@
       <c r="D5204" s="45"/>
       <c r="E5204" s="45"/>
     </row>
+    <row r="5217" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5217" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D5217" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5217" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5218" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5218" s="21"/>
+      <c r="D5218" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5218" s="43"/>
+    </row>
+    <row r="5219" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5219" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5219" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5219" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5220" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5220" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5220" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5220" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5221" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5221" s="9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D5221" s="10"/>
+      <c r="E5221" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5222" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5222" s="9">
+        <v>1.2</v>
+      </c>
+      <c r="D5222" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5222" s="11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5223" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5223" s="9">
+        <v>2.1</v>
+      </c>
+      <c r="D5223" s="10"/>
+      <c r="E5223" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5224" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5224" s="9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D5224" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5224" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5225" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5225" s="9">
+        <v>3.1</v>
+      </c>
+      <c r="D5225" s="10"/>
+      <c r="E5225" s="11" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5226" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5226" s="9">
+        <v>3.2</v>
+      </c>
+      <c r="D5226" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5226" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5227" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5227" s="9">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D5227" s="10"/>
+      <c r="E5227" s="11"/>
+    </row>
+    <row r="5228" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5228" s="9">
+        <v>4.2</v>
+      </c>
+      <c r="D5228" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5228" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5229" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5229" s="9">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="D5229" s="10"/>
+      <c r="E5229" s="22" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5230" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5230" s="9"/>
+      <c r="D5230" s="10"/>
+      <c r="E5230" s="22" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="5231" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5231" s="9"/>
+      <c r="D5231" s="10"/>
+      <c r="E5231" s="11" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5232" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5232" s="9"/>
+      <c r="D5232" s="10"/>
+      <c r="E5232" s="11" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5233" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5233" s="39">
+        <v>5.2</v>
+      </c>
+      <c r="D5233" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5233" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5234" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5234" s="9">
+        <v>6.1</v>
+      </c>
+      <c r="D5234" s="10"/>
+      <c r="E5234" s="22"/>
+    </row>
+    <row r="5235" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5235" s="9">
+        <v>6.2</v>
+      </c>
+      <c r="D5235" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5235" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5236" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5236" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5236" s="16"/>
+      <c r="E5236" s="17"/>
+    </row>
+    <row r="5238" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5238" s="45" t="e" vm="113">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D5238" s="45"/>
+      <c r="E5238" s="45"/>
+    </row>
+    <row r="5239" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5239" s="45"/>
+      <c r="D5239" s="45"/>
+      <c r="E5239" s="45"/>
+    </row>
+    <row r="5240" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5240" s="45"/>
+      <c r="D5240" s="45"/>
+      <c r="E5240" s="45"/>
+    </row>
+    <row r="5241" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5241" s="45"/>
+      <c r="D5241" s="45"/>
+      <c r="E5241" s="45"/>
+    </row>
+    <row r="5242" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5242" s="45"/>
+      <c r="D5242" s="45"/>
+      <c r="E5242" s="45"/>
+    </row>
+    <row r="5243" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5243" s="45"/>
+      <c r="D5243" s="45"/>
+      <c r="E5243" s="45"/>
+    </row>
+    <row r="5244" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5244" s="45"/>
+      <c r="D5244" s="45"/>
+      <c r="E5244" s="45"/>
+    </row>
+    <row r="5245" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5245" s="45"/>
+      <c r="D5245" s="45"/>
+      <c r="E5245" s="45"/>
+    </row>
+    <row r="5246" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5246" s="45"/>
+      <c r="D5246" s="45"/>
+      <c r="E5246" s="45"/>
+    </row>
+    <row r="5247" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5247" s="45"/>
+      <c r="D5247" s="45"/>
+      <c r="E5247" s="45"/>
+    </row>
+    <row r="5248" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5248" s="45"/>
+      <c r="D5248" s="45"/>
+      <c r="E5248" s="45"/>
+    </row>
+    <row r="5249" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5249" s="45"/>
+      <c r="D5249" s="45"/>
+      <c r="E5249" s="45"/>
+    </row>
+    <row r="5250" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5250" s="45"/>
+      <c r="D5250" s="45"/>
+      <c r="E5250" s="45"/>
+    </row>
+    <row r="5251" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5251" s="45"/>
+      <c r="D5251" s="45"/>
+      <c r="E5251" s="45"/>
+    </row>
   </sheetData>
-  <mergeCells count="348">
+  <mergeCells count="350">
     <mergeCell ref="B5142:E5142"/>
     <mergeCell ref="C5144:E5154"/>
     <mergeCell ref="D5171:E5171"/>
     <mergeCell ref="C5191:E5204"/>
+    <mergeCell ref="D5218:E5218"/>
+    <mergeCell ref="C5238:E5251"/>
     <mergeCell ref="D5077:E5077"/>
     <mergeCell ref="E5086:E5087"/>
     <mergeCell ref="C5095:E5106"/>

</xml_diff>